<commit_message>
continuing work on my instruction set
</commit_message>
<xml_diff>
--- a/res/instruction_set.xlsx
+++ b/res/instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukas\git\ArduOS\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35D2939-BE30-4742-950E-DFA0A8FC673C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2C42E2-B648-40D0-AFFE-BA73BFF86F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B2464EDA-0DBA-4918-93CA-197D58077369}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="163">
   <si>
     <t>Instr. ID</t>
   </si>
@@ -177,9 +177,6 @@
     <t>CMP</t>
   </si>
   <si>
-    <t>compare the value of two registers</t>
-  </si>
-  <si>
     <t>CMPI</t>
   </si>
   <si>
@@ -375,9 +372,6 @@
     <t>JMP</t>
   </si>
   <si>
-    <t>absolute jump to the address described by the unsigned integer combination of the values of registers A and B</t>
-  </si>
-  <si>
     <t>register B (less significant bytes)</t>
   </si>
   <si>
@@ -388,6 +382,138 @@
   </si>
   <si>
     <t>absolute jump to the address described by the 24-bit unsigned integer constant (little-endian)</t>
+  </si>
+  <si>
+    <t>absolute jump to the address described by the unsigned integer combination of the values of registers A and B (32-bit)</t>
+  </si>
+  <si>
+    <t>CALL</t>
+  </si>
+  <si>
+    <t>CALLI</t>
+  </si>
+  <si>
+    <t>jump to the address described by register A and B (32-bit unsigned integer, little-endian) and push PC to the stack</t>
+  </si>
+  <si>
+    <t>jump to the address described by constant (24-it unsigned integer, little-endian) and push PC to the stack</t>
+  </si>
+  <si>
+    <t>RET</t>
+  </si>
+  <si>
+    <t>Pop a value from the stack to PC (program counter), should be used in combination with CALL and/or CALLI</t>
+  </si>
+  <si>
+    <t>compare the values of two registers with each other</t>
+  </si>
+  <si>
+    <t>SEQ</t>
+  </si>
+  <si>
+    <t>SNE</t>
+  </si>
+  <si>
+    <t>SGR</t>
+  </si>
+  <si>
+    <t>SLE</t>
+  </si>
+  <si>
+    <t>SEQGR</t>
+  </si>
+  <si>
+    <t>SEQLE</t>
+  </si>
+  <si>
+    <t>Skip the next instruction if the equal flag is set</t>
+  </si>
+  <si>
+    <t>Skip the next instruction if the equal flag is not set</t>
+  </si>
+  <si>
+    <t>Skip the next instruction if the greater than flag is set</t>
+  </si>
+  <si>
+    <t>Skip the next instruction if the greater than flag is not set</t>
+  </si>
+  <si>
+    <t>Skip the next instruction if the equal or greater than flag is set</t>
+  </si>
+  <si>
+    <t>Skip the next instruction if the equal flag is set or the greater than flag is not set</t>
+  </si>
+  <si>
+    <t>BREQ</t>
+  </si>
+  <si>
+    <t>BRNE</t>
+  </si>
+  <si>
+    <t>BRGR</t>
+  </si>
+  <si>
+    <t>BRLE</t>
+  </si>
+  <si>
+    <t>BREQGR</t>
+  </si>
+  <si>
+    <t>BREQLE</t>
+  </si>
+  <si>
+    <t>Jump to the address described by bytes 1-3 (unsigned intger, 24-bit, little-endian) if the equal flag is set</t>
+  </si>
+  <si>
+    <t>Jump to the address described by bytes 1-3 (unsigned intger, 24-bit, little-endian) if the equal flag is not set</t>
+  </si>
+  <si>
+    <t>Jump to the address described by bytes 1-3 (unsigned intger, 24-bit, little-endian) if the greater than flag is set</t>
+  </si>
+  <si>
+    <t>Jump to the address described by bytes 1-3 (unsigned intger, 24-bit, little-endian) if the greater then flag is not set</t>
+  </si>
+  <si>
+    <t>Jump to the address described by bytes 1-3 (uint, 24-bit, little-endian) if equal flag or greater than flag is set</t>
+  </si>
+  <si>
+    <t>Jump to the address described by bytes 1-3 (uint, 24-bit, little-endian) if equal flag set or greater than flag is not set</t>
+  </si>
+  <si>
+    <t>IBREQ</t>
+  </si>
+  <si>
+    <t>IBRNE</t>
+  </si>
+  <si>
+    <t>IBRGR</t>
+  </si>
+  <si>
+    <t>IBRLE</t>
+  </si>
+  <si>
+    <t>IBREQGR</t>
+  </si>
+  <si>
+    <t>IBREQLE</t>
+  </si>
+  <si>
+    <t>Jump to the address described by registers A and B (32-bit uint, little-endian) if the equal flag is set</t>
+  </si>
+  <si>
+    <t>Jump to the address described by registers A and B (32-bit uint, little-endian) if the equal flag is not set</t>
+  </si>
+  <si>
+    <t>Jump to the address described by registers A and B (32-bit uint, little-endian) if the greater than flag is set</t>
+  </si>
+  <si>
+    <t>Jump to the address described by registers A and B (32-bit uint, little-endian) if the greater then flag is not set</t>
+  </si>
+  <si>
+    <t>Jump to the address described by registers A and B (32-bit uint, little-endian) if equal flag or greater than flag is set</t>
+  </si>
+  <si>
+    <t>Jump to address described by registers A and B (32-bit uint, little-endian) if equal flag set or greater than flag is not set</t>
   </si>
 </sst>
 </file>
@@ -578,7 +704,399 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="88">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1118,8 +1636,8 @@
   </sheetPr>
   <dimension ref="A1:H257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,7 +2090,7 @@
         <v>49</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>21</v>
@@ -1593,10 +2111,10 @@
         <v>0x12</v>
       </c>
       <c r="B20" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>21</v>
@@ -1617,10 +2135,10 @@
         <v>0x13</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>21</v>
@@ -1641,10 +2159,10 @@
         <v>0x14</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>21</v>
@@ -1668,7 +2186,7 @@
         <v>10</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>21</v>
@@ -1689,10 +2207,10 @@
         <v>0x16</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>21</v>
@@ -1713,10 +2231,10 @@
         <v>0x17</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>21</v>
@@ -1737,10 +2255,10 @@
         <v>0x18</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>21</v>
@@ -1761,10 +2279,10 @@
         <v>0x19</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>21</v>
@@ -1785,10 +2303,10 @@
         <v>0x1A</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>21</v>
@@ -1809,10 +2327,10 @@
         <v>0x1B</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>21</v>
@@ -1833,10 +2351,10 @@
         <v>0x1C</v>
       </c>
       <c r="B30" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>21</v>
@@ -1857,10 +2375,10 @@
         <v>0x1D</v>
       </c>
       <c r="B31" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>21</v>
@@ -1881,22 +2399,22 @@
         <v>0x1E</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1905,13 +2423,13 @@
         <v>0x1F</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>23</v>
@@ -1920,7 +2438,7 @@
         <v>23</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1929,22 +2447,22 @@
         <v>0x20</v>
       </c>
       <c r="B34" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1953,16 +2471,16 @@
         <v>0x21</v>
       </c>
       <c r="B35" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>23</v>
@@ -1977,10 +2495,10 @@
         <v>0x22</v>
       </c>
       <c r="B36" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>21</v>
@@ -2001,10 +2519,10 @@
         <v>0x23</v>
       </c>
       <c r="B37" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>21</v>
@@ -2025,19 +2543,19 @@
         <v>0x24</v>
       </c>
       <c r="B38" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>23</v>
@@ -2049,19 +2567,19 @@
         <v>0x25</v>
       </c>
       <c r="B39" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>23</v>
@@ -2073,10 +2591,10 @@
         <v>0x26</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>21</v>
@@ -2097,10 +2615,10 @@
         <v>0x27</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>21</v>
@@ -2121,10 +2639,10 @@
         <v>0x28</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>21</v>
@@ -2145,19 +2663,19 @@
         <v>0x29</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C43" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="F43" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G43" s="14" t="s">
         <v>23</v>
@@ -2169,10 +2687,10 @@
         <v>0x2A</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>21</v>
@@ -2193,13 +2711,13 @@
         <v>0x2B</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>23</v>
@@ -2217,10 +2735,10 @@
         <v>0x2C</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>21</v>
@@ -2241,19 +2759,19 @@
         <v>0x2D</v>
       </c>
       <c r="B47" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>114</v>
-      </c>
       <c r="D47" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>23</v>
@@ -2265,16 +2783,16 @@
         <v>0x2E</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>23</v>
@@ -2289,16 +2807,16 @@
         <v>0x2F</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D49" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>108</v>
@@ -2312,252 +2830,504 @@
         <f t="shared" si="1"/>
         <v>0x30</v>
       </c>
-      <c r="B50" s="13"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
+      <c r="B50" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x31</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
+      <c r="B51" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x32</v>
       </c>
-      <c r="B52" s="13"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
+      <c r="B52" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x33</v>
       </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
+      <c r="B53" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x34</v>
       </c>
-      <c r="B54" s="13"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
+      <c r="B54" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x35</v>
       </c>
-      <c r="B55" s="13"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
+      <c r="B55" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x36</v>
       </c>
-      <c r="B56" s="13"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
+      <c r="B56" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x37</v>
       </c>
-      <c r="B57" s="13"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
+      <c r="B57" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x38</v>
       </c>
-      <c r="B58" s="13"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
+      <c r="B58" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x39</v>
       </c>
-      <c r="B59" s="13"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
+      <c r="B59" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x3A</v>
       </c>
-      <c r="B60" s="13"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
+      <c r="B60" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x3B</v>
       </c>
-      <c r="B61" s="13"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
+      <c r="B61" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x3C</v>
       </c>
-      <c r="B62" s="13"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
+      <c r="B62" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x3D</v>
       </c>
-      <c r="B63" s="13"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
+      <c r="B63" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x3E</v>
       </c>
-      <c r="B64" s="13"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
+      <c r="B64" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x3F</v>
       </c>
-      <c r="B65" s="13"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
+      <c r="B65" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x40</v>
       </c>
-      <c r="B66" s="13"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
+      <c r="B66" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x41</v>
       </c>
-      <c r="B67" s="13"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
+      <c r="B67" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x42</v>
       </c>
-      <c r="B68" s="13"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
+      <c r="B68" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="str">
         <f t="shared" ref="A69:A132" si="2">CONCATENATE("0x", DEC2HEX(ROW()-2))</f>
         <v>0x43</v>
       </c>
-      <c r="B69" s="13"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
+      <c r="B69" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x44</v>
       </c>
-      <c r="B70" s="13"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
+      <c r="B70" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="str">
@@ -4805,117 +5575,313 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G31">
-    <cfRule type="containsText" dxfId="31" priority="27" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="87" priority="83" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G31)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="28" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="86" priority="84" operator="beginsWith" text="register">
       <formula>LEFT(G31,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G39 G50:G257">
-    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="bit copy store">
+  <conditionalFormatting sqref="G2:G39 G71:G257">
+    <cfRule type="containsText" dxfId="85" priority="81" operator="containsText" text="bit copy store">
       <formula>NOT(ISERROR(SEARCH("bit copy store",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="as specified in operand A">
+    <cfRule type="containsText" dxfId="84" priority="82" operator="containsText" text="as specified in operand A">
       <formula>NOT(ISERROR(SEARCH("as specified in operand A",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="equality, less/greater than">
+    <cfRule type="containsText" dxfId="83" priority="85" operator="containsText" text="equality, less/greater than">
       <formula>NOT(ISERROR(SEARCH("equality, less/greater than",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="carry">
+    <cfRule type="containsText" dxfId="82" priority="86" operator="containsText" text="carry">
       <formula>NOT(ISERROR(SEARCH("carry",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:F257">
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="bit no.">
+  <conditionalFormatting sqref="D2:F59 D71:F257 D65:E70">
+    <cfRule type="containsText" dxfId="81" priority="79" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="80" priority="80" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="35" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="79" priority="91" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D2)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="38" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="78" priority="94" operator="beginsWith" text="register">
       <formula>LEFT(D2,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35:G39">
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="77" priority="77" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G35)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="22" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="76" priority="78" operator="beginsWith" text="register">
       <formula>LEFT(G35,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="75" priority="73" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G44)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="74" priority="74" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G44)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="73" priority="75" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G44)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="20" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="72" priority="76" operator="beginsWith" text="register">
       <formula>LEFT(G44,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="71" priority="69" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="70" priority="70" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="69" priority="71" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G45)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="16" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="68" priority="72" operator="beginsWith" text="register">
       <formula>LEFT(G45,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46:G47">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="65" priority="67" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G46)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="12" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="64" priority="68" operator="beginsWith" text="register">
       <formula>LEFT(G46,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="63" priority="61" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="62" priority="62" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="61" priority="63" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G48)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="8" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="60" priority="64" operator="beginsWith" text="register">
       <formula>LEFT(G48,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49">
+    <cfRule type="containsText" dxfId="59" priority="57" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="58" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="59" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G49)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="56" priority="60" operator="beginsWith" text="register">
+      <formula>LEFT(G49,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G50">
+    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="55" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G50)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="52" priority="56" operator="beginsWith" text="register">
+      <formula>LEFT(G50,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G51">
+    <cfRule type="containsText" dxfId="51" priority="49" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G51)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="50" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G51)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="51" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G51)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="48" priority="52" operator="beginsWith" text="register">
+      <formula>LEFT(G51,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G52:G59">
+    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G52)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G52)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="47" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G52)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="44" priority="48" operator="beginsWith" text="register">
+      <formula>LEFT(G52,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60:F60">
+    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",D60)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",D60)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",D60)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="40" priority="44" operator="beginsWith" text="register">
+      <formula>LEFT(D60,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G60">
+    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G60)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G60)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G60)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="36" priority="40" operator="beginsWith" text="register">
+      <formula>LEFT(G60,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61:F61">
+    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",D61)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",D61)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",D61)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="32" priority="36" operator="beginsWith" text="register">
+      <formula>LEFT(D61,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G61">
+    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G61)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G61)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G61)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="28" priority="32" operator="beginsWith" text="register">
+      <formula>LEFT(G61,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62:F62">
+    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",D62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",D62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",D62)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="24" priority="28" operator="beginsWith" text="register">
+      <formula>LEFT(D62,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G62">
+    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G62)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G62)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="20" priority="24" operator="beginsWith" text="register">
+      <formula>LEFT(G62,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63:F63">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",D63)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",D63)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",D63)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="16" priority="20" operator="beginsWith" text="register">
+      <formula>LEFT(D63,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G63">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G63)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G63)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G63)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="12" priority="16" operator="beginsWith" text="register">
+      <formula>LEFT(G63,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D64:F64">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",D64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",D64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",D64)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="8" priority="12" operator="beginsWith" text="register">
+      <formula>LEFT(D64,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G64:G70">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G64)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="4" priority="8" operator="beginsWith" text="register">
+      <formula>LEFT(G64,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F65:F70">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",G49)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bit no.",F65)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",G49)))</formula>
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",F65)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",G49)))</formula>
+      <formula>NOT(ISERROR(SEARCH("byte of constant",F65)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="4" operator="beginsWith" text="register">
-      <formula>LEFT(G49,LEN("register"))="register"</formula>
+      <formula>LEFT(F65,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implemented all instructions up to RJMP (0x2F)
- minor changes to the instruction set
</commit_message>
<xml_diff>
--- a/res/instruction_set.xlsx
+++ b/res/instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukas\git\ArduOS\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6D7359-42F2-4F0A-8806-274D0FE8A58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28BB1FA-C07A-4128-9830-9F04671AFCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B2464EDA-0DBA-4918-93CA-197D58077369}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="249">
   <si>
     <t>Instr. ID</t>
   </si>
@@ -231,9 +231,6 @@
     <t>ASR</t>
   </si>
   <si>
-    <t>arithmetic shift right (same as LSR, but preserves the most significant bit)</t>
-  </si>
-  <si>
     <t>SWAP</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>save a bit from register A to the bit copy store (flag S)</t>
   </si>
   <si>
-    <t>bit no. (0 to 16)</t>
-  </si>
-  <si>
     <t>bit copy store</t>
   </si>
   <si>
@@ -766,6 +760,18 @@
   </si>
   <si>
     <t>Fill the whole screen with a constant color (values of bytes 1 and 2, little-endian)</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>set register A to ist one's complement</t>
+  </si>
+  <si>
+    <t>arithmetic shift right (same as RSR, but preserves the most significant bit)</t>
+  </si>
+  <si>
+    <t>bit no. (0 to 15)</t>
   </si>
 </sst>
 </file>
@@ -988,7 +994,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="274">
+  <dxfs count="137">
     <dxf>
       <fill>
         <patternFill>
@@ -1034,6 +1040,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1048,6 +1061,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1125,6 +1152,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1160,6 +1194,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1167,34 +1215,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1203,979 +1223,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3222,8 +2269,8 @@
   </sheetPr>
   <dimension ref="A1:H257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3601,10 +2648,10 @@
         <v>0xE</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>21</v>
@@ -3624,23 +2671,23 @@
         <f t="shared" si="1"/>
         <v>0xF</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>23</v>
+      <c r="B17" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3649,10 +2696,10 @@
         <v>0x10</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>21</v>
@@ -3673,22 +2720,22 @@
         <v>0x11</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>188</v>
+        <v>44</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>47</v>
+      <c r="E19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -3697,21 +2744,21 @@
         <v>0x12</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>22</v>
+      <c r="E20" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3721,19 +2768,19 @@
         <v>0x13</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>25</v>
+      <c r="E21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>47</v>
@@ -3745,22 +2792,22 @@
         <v>0x14</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>23</v>
+      <c r="E22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -3769,10 +2816,10 @@
         <v>0x15</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>21</v>
@@ -3783,7 +2830,7 @@
       <c r="F23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3793,16 +2840,16 @@
         <v>0x16</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>22</v>
+      <c r="E24" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>23</v>
@@ -3817,10 +2864,10 @@
         <v>0x17</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>21</v>
@@ -3841,10 +2888,10 @@
         <v>0x18</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>21</v>
@@ -3865,22 +2912,22 @@
         <v>0x19</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>23</v>
+      <c r="E27" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>11</v>
+      <c r="G27" s="14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3889,10 +2936,10 @@
         <v>0x1A</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>21</v>
@@ -3913,10 +2960,10 @@
         <v>0x1B</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>21</v>
@@ -3937,10 +2984,10 @@
         <v>0x1C</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>21</v>
@@ -3961,10 +3008,10 @@
         <v>0x1D</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>21</v>
@@ -3985,10 +3032,10 @@
         <v>0x1E</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>70</v>
+        <v>247</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>21</v>
@@ -3999,8 +3046,8 @@
       <c r="F32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>23</v>
+      <c r="G32" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -4009,13 +3056,13 @@
         <v>0x1F</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>23</v>
@@ -4023,8 +3070,8 @@
       <c r="F33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>74</v>
+      <c r="G33" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -4033,13 +3080,13 @@
         <v>0x20</v>
       </c>
       <c r="B34" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="D34" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>23</v>
@@ -4048,7 +3095,7 @@
         <v>23</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -4057,22 +3104,22 @@
         <v>0x21</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -4081,22 +3128,22 @@
         <v>0x22</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>79</v>
+        <v>248</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G36" s="4" t="s">
-        <v>23</v>
+      <c r="G36" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -4105,16 +3152,16 @@
         <v>0x23</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>22</v>
+        <v>248</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>23</v>
@@ -4129,19 +3176,19 @@
         <v>0x24</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>23</v>
@@ -4153,19 +3200,19 @@
         <v>0x25</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>23</v>
@@ -4177,19 +3224,19 @@
         <v>0x26</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>184</v>
+        <v>86</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>23</v>
@@ -4201,21 +3248,21 @@
         <v>0x27</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="14" t="s">
+      <c r="E41" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G41" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4225,10 +3272,10 @@
         <v>0x28</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>21</v>
@@ -4249,16 +3296,16 @@
         <v>0x29</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>22</v>
+      <c r="E43" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>23</v>
@@ -4272,20 +3319,20 @@
         <f t="shared" si="1"/>
         <v>0x2A</v>
       </c>
-      <c r="B44" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>101</v>
+      <c r="B44" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>105</v>
+        <v>21</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="G44" s="14" t="s">
         <v>23</v>
@@ -4296,22 +3343,22 @@
         <f t="shared" si="1"/>
         <v>0x2B</v>
       </c>
-      <c r="B45" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>98</v>
+      <c r="B45" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G45" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G45" s="14" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4320,14 +3367,14 @@
         <f t="shared" si="1"/>
         <v>0x2C</v>
       </c>
-      <c r="B46" s="16" t="s">
-        <v>97</v>
+      <c r="B46" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>107</v>
+        <v>21</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>23</v>
@@ -4344,14 +3391,14 @@
         <f t="shared" si="1"/>
         <v>0x2D</v>
       </c>
-      <c r="B47" s="13" t="s">
-        <v>96</v>
+      <c r="B47" s="16" t="s">
+        <v>95</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>23</v>
@@ -4369,19 +3416,19 @@
         <v>0x2E</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>104</v>
+        <v>21</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>23</v>
@@ -4393,19 +3440,19 @@
         <v>0x2F</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>23</v>
+        <v>101</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>23</v>
@@ -4417,19 +3464,19 @@
         <v>0x30</v>
       </c>
       <c r="B50" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="D50" s="3" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>23</v>
@@ -4441,19 +3488,19 @@
         <v>0x31</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>23</v>
+        <v>101</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>23</v>
@@ -4465,19 +3512,19 @@
         <v>0x32</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>105</v>
+        <v>22</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>23</v>
@@ -4489,19 +3536,19 @@
         <v>0x33</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>23</v>
+        <v>118</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>23</v>
@@ -4513,10 +3560,10 @@
         <v>0x34</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>23</v>
@@ -4537,10 +3584,10 @@
         <v>0x35</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>23</v>
@@ -4561,10 +3608,10 @@
         <v>0x36</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>23</v>
@@ -4585,10 +3632,10 @@
         <v>0x37</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>23</v>
@@ -4609,10 +3656,10 @@
         <v>0x38</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>23</v>
@@ -4633,10 +3680,10 @@
         <v>0x39</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>23</v>
@@ -4657,19 +3704,19 @@
         <v>0x3A</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>105</v>
+        <v>132</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>23</v>
@@ -4681,19 +3728,19 @@
         <v>0x3B</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E61" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>23</v>
@@ -4705,19 +3752,19 @@
         <v>0x3C</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E62" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>23</v>
@@ -4729,19 +3776,19 @@
         <v>0x3D</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E63" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>23</v>
@@ -4753,19 +3800,19 @@
         <v>0x3E</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E64" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>23</v>
@@ -4777,19 +3824,19 @@
         <v>0x3F</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E65" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F65" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>23</v>
@@ -4801,19 +3848,19 @@
         <v>0x40</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>23</v>
+        <v>101</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>23</v>
@@ -4825,10 +3872,10 @@
         <v>0x41</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>21</v>
@@ -4849,10 +3896,10 @@
         <v>0x42</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>21</v>
@@ -4873,10 +3920,10 @@
         <v>0x43</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>21</v>
@@ -4897,10 +3944,10 @@
         <v>0x44</v>
       </c>
       <c r="B70" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>21</v>
@@ -4921,10 +3968,10 @@
         <v>0x45</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>21</v>
@@ -4945,10 +3992,10 @@
         <v>0x46</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>21</v>
@@ -4956,8 +4003,8 @@
       <c r="E72" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F72" s="3" t="s">
-        <v>161</v>
+      <c r="F72" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>23</v>
@@ -4968,20 +4015,20 @@
         <f t="shared" si="2"/>
         <v>0x47</v>
       </c>
-      <c r="B73" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="D73" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>23</v>
+      <c r="B73" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>23</v>
@@ -4993,16 +4040,16 @@
         <v>0x48</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="E74" s="17" t="s">
-        <v>171</v>
+        <v>21</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F74" s="4" t="s">
         <v>23</v>
@@ -5016,17 +4063,17 @@
         <f t="shared" si="2"/>
         <v>0x49</v>
       </c>
-      <c r="B75" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>23</v>
+      <c r="B75" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="D75" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="E75" s="17" t="s">
+        <v>169</v>
       </c>
       <c r="F75" s="4" t="s">
         <v>23</v>
@@ -5041,13 +4088,13 @@
         <v>0x4A</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>23</v>
@@ -5065,13 +4112,13 @@
         <v>0x4B</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>23</v>
@@ -5089,16 +4136,16 @@
         <v>0x4C</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E78" s="3" t="s">
-        <v>22</v>
+      <c r="E78" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F78" s="4" t="s">
         <v>23</v>
@@ -5113,16 +4160,16 @@
         <v>0x4D</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>171</v>
+        <v>22</v>
       </c>
       <c r="F79" s="4" t="s">
         <v>23</v>
@@ -5137,16 +4184,16 @@
         <v>0x4E</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>23</v>
+        <v>100</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="F80" s="4" t="s">
         <v>23</v>
@@ -5161,13 +4208,13 @@
         <v>0x4F</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>23</v>
@@ -5184,17 +4231,17 @@
         <f t="shared" si="2"/>
         <v>0x50</v>
       </c>
-      <c r="B82" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="D82" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E82" s="18" t="s">
-        <v>22</v>
+      <c r="B82" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F82" s="4" t="s">
         <v>23</v>
@@ -5208,17 +4255,17 @@
         <f t="shared" si="2"/>
         <v>0x51</v>
       </c>
-      <c r="B83" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>23</v>
+      <c r="B83" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C83" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D83" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="F83" s="4" t="s">
         <v>23</v>
@@ -5233,13 +4280,13 @@
         <v>0x52</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>23</v>
@@ -5257,16 +4304,16 @@
         <v>0x53</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>187</v>
+        <v>100</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F85" s="4" t="s">
         <v>23</v>
@@ -5281,19 +4328,19 @@
         <v>0x54</v>
       </c>
       <c r="B86" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E86" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>105</v>
+      <c r="F86" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>23</v>
@@ -5305,19 +4352,19 @@
         <v>0x55</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>161</v>
+        <v>103</v>
       </c>
       <c r="G87" s="4" t="s">
         <v>23</v>
@@ -5329,10 +4376,10 @@
         <v>0x56</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>21</v>
@@ -5341,7 +4388,7 @@
         <v>22</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>23</v>
@@ -5353,10 +4400,10 @@
         <v>0x57</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>21</v>
@@ -5365,7 +4412,7 @@
         <v>22</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G89" s="4" t="s">
         <v>23</v>
@@ -5377,10 +4424,10 @@
         <v>0x58</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>21</v>
@@ -5389,7 +4436,7 @@
         <v>22</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>23</v>
@@ -5401,10 +4448,10 @@
         <v>0x59</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>21</v>
@@ -5413,7 +4460,7 @@
         <v>22</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>23</v>
@@ -5425,10 +4472,10 @@
         <v>0x5A</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>21</v>
@@ -5436,8 +4483,8 @@
       <c r="E92" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F92" s="4" t="s">
-        <v>23</v>
+      <c r="F92" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="G92" s="4" t="s">
         <v>23</v>
@@ -5449,16 +4496,16 @@
         <v>0x5B</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E93" s="4" t="s">
-        <v>23</v>
+      <c r="E93" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F93" s="4" t="s">
         <v>23</v>
@@ -5473,13 +4520,13 @@
         <v>0x5C</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>23</v>
+        <v>203</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E94" s="4" t="s">
         <v>23</v>
@@ -5497,10 +4544,10 @@
         <v>0x5D</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>23</v>
@@ -5521,13 +4568,13 @@
         <v>0x5E</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>21</v>
+        <v>207</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>23</v>
@@ -5545,13 +4592,13 @@
         <v>0x5F</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>23</v>
+        <v>209</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>23</v>
@@ -5568,20 +4615,20 @@
         <f t="shared" si="2"/>
         <v>0x60</v>
       </c>
-      <c r="B98" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="C98" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="D98" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>222</v>
+      <c r="B98" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="G98" s="4" t="s">
         <v>23</v>
@@ -5593,22 +4640,22 @@
         <v>0x61</v>
       </c>
       <c r="B99" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="C99" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="C99" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>102</v>
+      <c r="D99" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G99" s="22" t="s">
-        <v>80</v>
+        <v>220</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -5617,22 +4664,22 @@
         <v>0x62</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="D100" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E100" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F100" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G100" s="20" t="s">
-        <v>23</v>
+        <v>225</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G100" s="22" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -5641,13 +4688,13 @@
         <v>0x63</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="C101" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="D101" t="s">
-        <v>21</v>
+        <v>210</v>
+      </c>
+      <c r="C101" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="E101" s="20" t="s">
         <v>23</v>
@@ -5665,13 +4712,13 @@
         <v>0x64</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C102" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="D102" s="14" t="s">
-        <v>23</v>
+        <v>224</v>
+      </c>
+      <c r="D102" t="s">
+        <v>21</v>
       </c>
       <c r="E102" s="20" t="s">
         <v>23</v>
@@ -5689,10 +4736,10 @@
         <v>0x65</v>
       </c>
       <c r="B103" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="C103" s="21" t="s">
         <v>229</v>
-      </c>
-      <c r="C103" s="21" t="s">
-        <v>230</v>
       </c>
       <c r="D103" s="14" t="s">
         <v>23</v>
@@ -5712,22 +4759,22 @@
         <f t="shared" si="2"/>
         <v>0x66</v>
       </c>
-      <c r="B104" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D104" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E104" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F104" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G104" s="4" t="s">
+      <c r="B104" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="C104" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="D104" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E104" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F104" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G104" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5737,13 +4784,13 @@
         <v>0x67</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>102</v>
+        <v>213</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>23</v>
@@ -5761,13 +4808,13 @@
         <v>0x68</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>23</v>
@@ -5785,19 +4832,19 @@
         <v>0x69</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="D107" t="s">
-        <v>21</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="F107" s="3" t="s">
-        <v>222</v>
+        <v>217</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="G107" s="4" t="s">
         <v>23</v>
@@ -5808,20 +4855,23 @@
         <f t="shared" si="2"/>
         <v>0x6A</v>
       </c>
-      <c r="B108" s="16" t="s">
+      <c r="B108" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D108" t="s">
+        <v>21</v>
+      </c>
+      <c r="E108" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="C108" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D108" t="s">
-        <v>236</v>
-      </c>
-      <c r="E108" s="23" t="s">
-        <v>238</v>
-      </c>
       <c r="F108" s="3" t="s">
-        <v>187</v>
+        <v>220</v>
+      </c>
+      <c r="G108" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -5829,23 +4879,20 @@
         <f t="shared" si="2"/>
         <v>0x6B</v>
       </c>
-      <c r="B109" s="13" t="s">
-        <v>232</v>
+      <c r="B109" s="16" t="s">
+        <v>235</v>
       </c>
       <c r="C109" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D109" t="s">
         <v>234</v>
       </c>
-      <c r="D109" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E109" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F109" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G109" s="4" t="s">
-        <v>23</v>
+      <c r="E109" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -5853,12 +4900,24 @@
         <f t="shared" si="2"/>
         <v>0x6C</v>
       </c>
-      <c r="B110" s="13"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3"/>
-      <c r="F110" s="3"/>
-      <c r="G110" s="3"/>
+      <c r="B110" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="str">
@@ -7625,500 +6684,500 @@
       <c r="G257" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G32">
-    <cfRule type="containsText" dxfId="273" priority="168" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",G32)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="272" priority="169" operator="beginsWith" text="register">
-      <formula>LEFT(G32,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="G33">
+    <cfRule type="containsText" dxfId="136" priority="168" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G33)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="135" priority="169" operator="beginsWith" text="register">
+      <formula>LEFT(G33,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G40 G109:G257">
-    <cfRule type="containsText" dxfId="271" priority="167" operator="containsText" text="as specified in operand A">
+  <conditionalFormatting sqref="G110:G257 G2:G41">
+    <cfRule type="containsText" dxfId="134" priority="167" operator="containsText" text="as specified in operand A">
       <formula>NOT(ISERROR(SEARCH("as specified in operand A",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="270" priority="170" operator="containsText" text="equality, less/greater than">
+    <cfRule type="containsText" dxfId="133" priority="170" operator="containsText" text="equality, less/greater than">
       <formula>NOT(ISERROR(SEARCH("equality, less/greater than",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="269" priority="171" operator="containsText" text="carry">
+    <cfRule type="containsText" dxfId="132" priority="171" operator="containsText" text="carry">
       <formula>NOT(ISERROR(SEARCH("carry",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G36:G40">
-    <cfRule type="containsText" dxfId="268" priority="162" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",G36)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="267" priority="163" operator="beginsWith" text="register">
-      <formula>LEFT(G36,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="G37:G41">
+    <cfRule type="containsText" dxfId="131" priority="162" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G37)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="130" priority="163" operator="beginsWith" text="register">
+      <formula>LEFT(G37,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G45 G73:G75">
-    <cfRule type="containsText" dxfId="266" priority="158" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",G45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="265" priority="159" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",G45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="264" priority="160" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",G45)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="263" priority="161" operator="beginsWith" text="register">
-      <formula>LEFT(G45,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="G46 G74:G76">
+    <cfRule type="containsText" dxfId="129" priority="158" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="128" priority="159" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="127" priority="160" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G46)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="126" priority="161" operator="beginsWith" text="register">
+      <formula>LEFT(G46,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
-    <cfRule type="containsText" dxfId="262" priority="154" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",G46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="155" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",G46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="260" priority="156" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",G46)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="259" priority="157" operator="beginsWith" text="register">
-      <formula>LEFT(G46,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="G47">
+    <cfRule type="containsText" dxfId="125" priority="154" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G47)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="124" priority="155" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G47)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="123" priority="156" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G47)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="122" priority="157" operator="beginsWith" text="register">
+      <formula>LEFT(G47,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G47:G48">
-    <cfRule type="containsText" dxfId="258" priority="150" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",G47)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="257" priority="151" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",G47)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="256" priority="152" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",G47)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="255" priority="153" operator="beginsWith" text="register">
-      <formula>LEFT(G47,LEN("register"))="register"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G49">
-    <cfRule type="containsText" dxfId="254" priority="146" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",G49)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="253" priority="147" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",G49)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="252" priority="148" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",G49)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="251" priority="149" operator="beginsWith" text="register">
-      <formula>LEFT(G49,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="G48:G49">
+    <cfRule type="containsText" dxfId="121" priority="150" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="120" priority="151" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="119" priority="152" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G48)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="118" priority="153" operator="beginsWith" text="register">
+      <formula>LEFT(G48,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="containsText" dxfId="250" priority="142" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="117" priority="146" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="249" priority="143" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="116" priority="147" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="248" priority="144" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="115" priority="148" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G50)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="247" priority="145" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="114" priority="149" operator="beginsWith" text="register">
       <formula>LEFT(G50,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="246" priority="138" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="113" priority="142" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="245" priority="139" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="112" priority="143" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="244" priority="140" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="111" priority="144" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G51)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="243" priority="141" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="110" priority="145" operator="beginsWith" text="register">
       <formula>LEFT(G51,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="containsText" dxfId="242" priority="134" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="109" priority="138" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="241" priority="135" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="108" priority="139" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="240" priority="136" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="107" priority="140" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G52)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="239" priority="137" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="106" priority="141" operator="beginsWith" text="register">
       <formula>LEFT(G52,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G53:G60">
-    <cfRule type="containsText" dxfId="238" priority="130" operator="containsText" text="bit no.">
+  <conditionalFormatting sqref="G53">
+    <cfRule type="containsText" dxfId="105" priority="134" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="237" priority="131" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="104" priority="135" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="236" priority="132" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="103" priority="136" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G53)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="235" priority="133" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="102" priority="137" operator="beginsWith" text="register">
       <formula>LEFT(G53,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D61:F61">
-    <cfRule type="containsText" dxfId="234" priority="126" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",D61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="233" priority="127" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",D61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="232" priority="128" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",D61)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="231" priority="129" operator="beginsWith" text="register">
-      <formula>LEFT(D61,LEN("register"))="register"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G61">
-    <cfRule type="containsText" dxfId="230" priority="122" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",G61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="229" priority="123" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",G61)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="228" priority="124" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",G61)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="227" priority="125" operator="beginsWith" text="register">
-      <formula>LEFT(G61,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="G54:G61">
+    <cfRule type="containsText" dxfId="101" priority="130" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="131" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="99" priority="132" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G54)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="98" priority="133" operator="beginsWith" text="register">
+      <formula>LEFT(G54,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62:F62">
-    <cfRule type="containsText" dxfId="226" priority="118" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="97" priority="126" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="225" priority="119" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="96" priority="127" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="224" priority="120" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="95" priority="128" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D62)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="223" priority="121" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="94" priority="129" operator="beginsWith" text="register">
       <formula>LEFT(D62,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="containsText" dxfId="222" priority="114" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="93" priority="122" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="221" priority="115" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="92" priority="123" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="220" priority="116" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="91" priority="124" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G62)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="219" priority="117" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="90" priority="125" operator="beginsWith" text="register">
       <formula>LEFT(G62,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63:F63">
-    <cfRule type="containsText" dxfId="218" priority="110" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="89" priority="118" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="217" priority="111" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="88" priority="119" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="216" priority="112" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="87" priority="120" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D63)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="215" priority="113" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="86" priority="121" operator="beginsWith" text="register">
       <formula>LEFT(D63,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G63">
-    <cfRule type="containsText" dxfId="214" priority="106" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="85" priority="114" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="107" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="84" priority="115" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="212" priority="108" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="83" priority="116" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G63)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="211" priority="109" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="82" priority="117" operator="beginsWith" text="register">
       <formula>LEFT(G63,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64:F64">
-    <cfRule type="containsText" dxfId="210" priority="102" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="81" priority="110" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="103" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="80" priority="111" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="208" priority="104" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="79" priority="112" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D64)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="207" priority="105" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="78" priority="113" operator="beginsWith" text="register">
       <formula>LEFT(D64,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G64">
-    <cfRule type="containsText" dxfId="206" priority="98" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="77" priority="106" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="99" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="76" priority="107" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="100" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="75" priority="108" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G64)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="203" priority="101" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="74" priority="109" operator="beginsWith" text="register">
       <formula>LEFT(G64,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:F65">
-    <cfRule type="containsText" dxfId="202" priority="94" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="73" priority="102" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="95" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="72" priority="103" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="200" priority="96" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="71" priority="104" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D65)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="199" priority="97" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="70" priority="105" operator="beginsWith" text="register">
       <formula>LEFT(D65,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G65:G72">
-    <cfRule type="containsText" dxfId="198" priority="90" operator="containsText" text="bit no.">
+  <conditionalFormatting sqref="G65">
+    <cfRule type="containsText" dxfId="69" priority="98" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="91" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="68" priority="99" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="92" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="67" priority="100" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G65)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="195" priority="93" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="66" priority="101" operator="beginsWith" text="register">
       <formula>LEFT(G65,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F66:F71">
-    <cfRule type="containsText" dxfId="194" priority="86" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",F66)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="87" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",F66)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="88" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",F66)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="191" priority="89" operator="beginsWith" text="register">
-      <formula>LEFT(F66,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="D66:F66">
+    <cfRule type="containsText" dxfId="65" priority="94" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",D66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="95" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",D66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="96" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",D66)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="62" priority="97" operator="beginsWith" text="register">
+      <formula>LEFT(D66,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G76:G79">
-    <cfRule type="containsText" dxfId="190" priority="78" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",G76)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="79" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",G76)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="188" priority="80" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",G76)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="187" priority="81" operator="beginsWith" text="register">
-      <formula>LEFT(G76,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="G66:G73">
+    <cfRule type="containsText" dxfId="61" priority="90" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="91" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="59" priority="92" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G66)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="58" priority="93" operator="beginsWith" text="register">
+      <formula>LEFT(G66,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G92">
-    <cfRule type="containsText" dxfId="186" priority="58" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",G92)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="59" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",G92)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="60" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",G92)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="183" priority="61" operator="beginsWith" text="register">
-      <formula>LEFT(G92,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="F67:F72">
+    <cfRule type="containsText" dxfId="57" priority="86" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",F67)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="87" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",F67)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="88" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",F67)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="54" priority="89" operator="beginsWith" text="register">
+      <formula>LEFT(F67,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E93:G96">
-    <cfRule type="containsText" dxfId="182" priority="54" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",E93)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="55" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",E93)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="56" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",E93)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="179" priority="57" operator="beginsWith" text="register">
-      <formula>LEFT(E93,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="G77:G80">
+    <cfRule type="containsText" dxfId="53" priority="78" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G77)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="79" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G77)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="80" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G77)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="50" priority="81" operator="beginsWith" text="register">
+      <formula>LEFT(G77,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D94:D95">
-    <cfRule type="containsText" dxfId="178" priority="50" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",D94)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="51" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",D94)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="176" priority="52" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",D94)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="175" priority="53" operator="beginsWith" text="register">
-      <formula>LEFT(D94,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="G93">
+    <cfRule type="containsText" dxfId="49" priority="58" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G93)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="59" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G93)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="60" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G93)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="46" priority="61" operator="beginsWith" text="register">
+      <formula>LEFT(G93,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E94:G97">
+    <cfRule type="containsText" dxfId="45" priority="54" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",E94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="55" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",E94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="56" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",E94)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="42" priority="57" operator="beginsWith" text="register">
+      <formula>LEFT(E94,LEN("register"))="register"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D95:D96">
+    <cfRule type="containsText" dxfId="41" priority="50" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",D95)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="51" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",D95)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="52" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",D95)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="38" priority="53" operator="beginsWith" text="register">
+      <formula>LEFT(D95,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:F257">
-    <cfRule type="beginsWith" dxfId="174" priority="41" operator="beginsWith" text="byte ">
+    <cfRule type="beginsWith" dxfId="37" priority="41" operator="beginsWith" text="byte ">
       <formula>LEFT(D2,LEN("byte "))="byte "</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="164" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="36" priority="164" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="165" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="35" priority="165" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="176" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="34" priority="176" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D2)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="137" priority="179" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="33" priority="179" operator="beginsWith" text="register">
       <formula>LEFT(D2,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E98:F98">
-    <cfRule type="containsText" dxfId="173" priority="37" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",E98)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="38" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",E98)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="39" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",E98)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="170" priority="40" operator="beginsWith" text="register">
-      <formula>LEFT(E98,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="E99:F99">
+    <cfRule type="containsText" dxfId="32" priority="37" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",E99)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="38" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",E99)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="39" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",E99)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="29" priority="40" operator="beginsWith" text="register">
+      <formula>LEFT(E99,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E98:F98">
-    <cfRule type="beginsWith" dxfId="169" priority="36" operator="beginsWith" text="byte ">
-      <formula>LEFT(E98,LEN("byte "))="byte "</formula>
+  <conditionalFormatting sqref="E99:F99">
+    <cfRule type="beginsWith" dxfId="28" priority="36" operator="beginsWith" text="byte ">
+      <formula>LEFT(E99,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D99:F99">
-    <cfRule type="containsText" dxfId="168" priority="32" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",D99)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="167" priority="33" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",D99)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="34" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",D99)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="165" priority="35" operator="beginsWith" text="register">
-      <formula>LEFT(D99,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="D100:F100">
+    <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",D100)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="33" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",D100)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="34" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",D100)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="24" priority="35" operator="beginsWith" text="register">
+      <formula>LEFT(D100,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D99:F99">
-    <cfRule type="beginsWith" dxfId="164" priority="31" operator="beginsWith" text="byte ">
-      <formula>LEFT(D99,LEN("byte "))="byte "</formula>
+  <conditionalFormatting sqref="D100:F100">
+    <cfRule type="beginsWith" dxfId="23" priority="31" operator="beginsWith" text="byte ">
+      <formula>LEFT(D100,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G104:G106 G109:G257 G2:G101">
-    <cfRule type="containsText" dxfId="163" priority="166" operator="containsText" text="bit copy store">
+  <conditionalFormatting sqref="G105:G107 G110:G257 G2:G102">
+    <cfRule type="containsText" dxfId="22" priority="166" operator="containsText" text="bit copy store">
       <formula>NOT(ISERROR(SEARCH("bit copy store",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G102:G103">
-    <cfRule type="containsText" dxfId="162" priority="30" operator="containsText" text="bit copy store">
-      <formula>NOT(ISERROR(SEARCH("bit copy store",G102)))</formula>
+  <conditionalFormatting sqref="G103:G104">
+    <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text="bit copy store">
+      <formula>NOT(ISERROR(SEARCH("bit copy store",G103)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107">
-    <cfRule type="containsText" dxfId="161" priority="25" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",G107)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="26" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",G107)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="28" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",G107)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="158" priority="29" operator="beginsWith" text="register">
-      <formula>LEFT(G107,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="G108">
+    <cfRule type="containsText" dxfId="20" priority="25" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",G108)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="26" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G108)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="28" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G108)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="17" priority="29" operator="beginsWith" text="register">
+      <formula>LEFT(G108,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E107:F107 F108">
-    <cfRule type="beginsWith" dxfId="157" priority="6" operator="beginsWith" text="byte ">
-      <formula>LEFT(E107,LEN("byte "))="byte "</formula>
+  <conditionalFormatting sqref="E108:F108 F109">
+    <cfRule type="beginsWith" dxfId="16" priority="6" operator="beginsWith" text="byte ">
+      <formula>LEFT(E108,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107">
-    <cfRule type="containsText" dxfId="156" priority="27" operator="containsText" text="bit copy store">
-      <formula>NOT(ISERROR(SEARCH("bit copy store",G107)))</formula>
+  <conditionalFormatting sqref="G108">
+    <cfRule type="containsText" dxfId="15" priority="27" operator="containsText" text="bit copy store">
+      <formula>NOT(ISERROR(SEARCH("bit copy store",G108)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E109:G109">
-    <cfRule type="containsText" dxfId="155" priority="12" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",E109)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="13" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",E109)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="15" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",E109)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="152" priority="16" operator="beginsWith" text="register">
-      <formula>LEFT(E109,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="E110:G110">
+    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",E110)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",E110)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",E110)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="11" priority="16" operator="beginsWith" text="register">
+      <formula>LEFT(E110,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E109:F109">
-    <cfRule type="beginsWith" dxfId="151" priority="11" operator="beginsWith" text="byte ">
-      <formula>LEFT(E109,LEN("byte "))="byte "</formula>
+  <conditionalFormatting sqref="E110:F110">
+    <cfRule type="beginsWith" dxfId="10" priority="11" operator="beginsWith" text="byte ">
+      <formula>LEFT(E110,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G109">
-    <cfRule type="containsText" dxfId="150" priority="14" operator="containsText" text="bit copy store">
-      <formula>NOT(ISERROR(SEARCH("bit copy store",G109)))</formula>
+  <conditionalFormatting sqref="G110">
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="bit copy store">
+      <formula>NOT(ISERROR(SEARCH("bit copy store",G110)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E107:F107 F108">
-    <cfRule type="containsText" dxfId="149" priority="7" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",E107)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="8" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",E107)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="9" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",E107)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="146" priority="10" operator="beginsWith" text="register">
-      <formula>LEFT(E107,LEN("register"))="register"</formula>
+  <conditionalFormatting sqref="E108:F108 F109">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="bit no.">
+      <formula>NOT(ISERROR(SEARCH("bit no.",E108)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="flag name/no.">
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",E108)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="byte of constant">
+      <formula>NOT(ISERROR(SEARCH("byte of constant",E108)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="5" priority="10" operator="beginsWith" text="register">
+      <formula>LEFT(E108,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16:F16">
-    <cfRule type="containsText" dxfId="145" priority="4" operator="containsText" text="byte of constant">
+  <conditionalFormatting sqref="E16:F17">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16:F16">
-    <cfRule type="beginsWith" dxfId="144" priority="1" operator="beginsWith" text="byte ">
+  <conditionalFormatting sqref="E16:F17">
+    <cfRule type="beginsWith" dxfId="3" priority="1" operator="beginsWith" text="byte ">
       <formula>LEFT(E16,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16:F16">
-    <cfRule type="containsText" dxfId="143" priority="2" operator="containsText" text="bit no.">
+  <conditionalFormatting sqref="E16:F17">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="3" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",E16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="141" priority="5" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="0" priority="5" operator="beginsWith" text="register">
       <formula>LEFT(E16,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
implemented all instructions up to TOUTI (0x53)
</commit_message>
<xml_diff>
--- a/res/instruction_set.xlsx
+++ b/res/instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukas\git\ArduOS\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28BB1FA-C07A-4128-9830-9F04671AFCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DC77D5-8EDA-4BD6-A0CE-1A07E99D4406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B2464EDA-0DBA-4918-93CA-197D58077369}"/>
   </bookViews>
@@ -2269,8 +2269,8 @@
   </sheetPr>
   <dimension ref="A1:H257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
implemented almost all instructions
not yet implemented:
- SET (0x69)
- SETI (0x6A)
- GET (0x6B)
- GETI (0x6C)
</commit_message>
<xml_diff>
--- a/res/instruction_set.xlsx
+++ b/res/instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukas\git\ArduOS\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DC77D5-8EDA-4BD6-A0CE-1A07E99D4406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4B75AE-D231-499D-99A7-DBAA53AF6375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B2464EDA-0DBA-4918-93CA-197D58077369}"/>
   </bookViews>
@@ -579,9 +579,6 @@
     <t>IMGI</t>
   </si>
   <si>
-    <t>Draw an image file with it's path specified by a null-terminated string at a memory address specified by bytes 1-3</t>
-  </si>
-  <si>
     <t>register B (most significant bytes)</t>
   </si>
   <si>
@@ -597,9 +594,6 @@
     <t>FEXISTS</t>
   </si>
   <si>
-    <t>Draw an image file with it's path specified by a null-terminated string at a memory address specified by registers A &amp; B</t>
-  </si>
-  <si>
     <t>Set register A to 1, if file with path located at memory address specified by reg B &amp; C exists (null-terminated string)</t>
   </si>
   <si>
@@ -630,15 +624,9 @@
     <t>FNAME</t>
   </si>
   <si>
-    <t>Set register A to the byte value of the Xth char in the filename (X = value of rehister B)</t>
-  </si>
-  <si>
     <t>FAV</t>
   </si>
   <si>
-    <t>Set register A to 1, if there a bytes available to be read from</t>
-  </si>
-  <si>
     <t>FCLOS</t>
   </si>
   <si>
@@ -693,9 +681,6 @@
     <t>go to a position in the file specified by registers B and C (little-endian, unsigned int), set reg A to 1 on success, to 0 on failure</t>
   </si>
   <si>
-    <t>save the size of the currently open file to registers 0 and 1 (little endian, unsigned long)</t>
-  </si>
-  <si>
     <t>FISDIR</t>
   </si>
   <si>
@@ -714,9 +699,6 @@
     <t>return to the first file in the directory (opens the first file on next call to FNEXT)</t>
   </si>
   <si>
-    <t>opens the next file in the current directory (sets bit copy store to on success, to 0 on failure); will always switch the current file</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
@@ -772,6 +754,24 @@
   </si>
   <si>
     <t>bit no. (0 to 15)</t>
+  </si>
+  <si>
+    <t>Draw an image file with it's path specified by a null-terminated string at a memory address specified by registers A &amp; B at the cursor position</t>
+  </si>
+  <si>
+    <t>Draw an image file with it's path specified by a null-terminated string at a memory address specified by bytes 1-3 at the current cursor position</t>
+  </si>
+  <si>
+    <t>Set register A to the byte value of the Xth char in the filename (X = value of register B)</t>
+  </si>
+  <si>
+    <t>Set register A to the number of bytes available to read</t>
+  </si>
+  <si>
+    <t>GETI</t>
+  </si>
+  <si>
+    <t>opens the next file in the current directory (sets bit copy store to 1 on success, to 0 on failure); will always switch the current file</t>
   </si>
 </sst>
 </file>
@@ -951,7 +951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -990,6 +990,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2269,8 +2270,8 @@
   </sheetPr>
   <dimension ref="A1:H257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2648,10 +2649,10 @@
         <v>0xE</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>21</v>
@@ -2672,10 +2673,10 @@
         <v>0xF</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>21</v>
@@ -2747,7 +2748,7 @@
         <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>21</v>
@@ -2771,7 +2772,7 @@
         <v>48</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>21</v>
@@ -2795,7 +2796,7 @@
         <v>49</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>21</v>
@@ -3035,7 +3036,7 @@
         <v>67</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>21</v>
@@ -3137,7 +3138,7 @@
         <v>21</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>23</v>
@@ -3161,7 +3162,7 @@
         <v>21</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>23</v>
@@ -4040,10 +4041,10 @@
         <v>0x48</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D74" s="17" t="s">
         <v>21</v>
@@ -4064,10 +4065,10 @@
         <v>0x49</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D75" s="17" t="s">
         <v>100</v>
@@ -4331,13 +4332,13 @@
         <v>181</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>190</v>
+        <v>243</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>23</v>
@@ -4355,7 +4356,7 @@
         <v>183</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>184</v>
+        <v>244</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>100</v>
@@ -4376,10 +4377,10 @@
         <v>0x56</v>
       </c>
       <c r="B88" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>21</v>
@@ -4400,10 +4401,10 @@
         <v>0x57</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>21</v>
@@ -4424,10 +4425,10 @@
         <v>0x58</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>21</v>
@@ -4448,10 +4449,10 @@
         <v>0x59</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>21</v>
@@ -4472,10 +4473,10 @@
         <v>0x5A</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>21</v>
@@ -4496,10 +4497,10 @@
         <v>0x5B</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>201</v>
+        <v>245</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>21</v>
@@ -4520,10 +4521,10 @@
         <v>0x5C</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>203</v>
+        <v>246</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>21</v>
@@ -4544,10 +4545,10 @@
         <v>0x5D</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>23</v>
@@ -4568,10 +4569,10 @@
         <v>0x5E</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>23</v>
@@ -4592,10 +4593,10 @@
         <v>0x5F</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>21</v>
@@ -4616,10 +4617,10 @@
         <v>0x60</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>23</v>
@@ -4640,10 +4641,10 @@
         <v>0x61</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D99" s="19" t="s">
         <v>21</v>
@@ -4652,7 +4653,7 @@
         <v>22</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G99" s="4" t="s">
         <v>23</v>
@@ -4664,10 +4665,10 @@
         <v>0x62</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>100</v>
@@ -4688,13 +4689,13 @@
         <v>0x63</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="C101" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>23</v>
+        <v>218</v>
+      </c>
+      <c r="C101" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="D101" t="s">
+        <v>21</v>
       </c>
       <c r="E101" s="20" t="s">
         <v>23</v>
@@ -4712,13 +4713,13 @@
         <v>0x64</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C102" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="D102" t="s">
-        <v>21</v>
+        <v>248</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="E102" s="20" t="s">
         <v>23</v>
@@ -4736,10 +4737,10 @@
         <v>0x65</v>
       </c>
       <c r="B103" s="16" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C103" s="21" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D103" s="14" t="s">
         <v>23</v>
@@ -4759,22 +4760,22 @@
         <f t="shared" si="2"/>
         <v>0x66</v>
       </c>
-      <c r="B104" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="C104" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="D104" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E104" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F104" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G104" s="20" t="s">
+      <c r="B104" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G104" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4784,13 +4785,13 @@
         <v>0x67</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>21</v>
+        <v>211</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>23</v>
@@ -4808,13 +4809,13 @@
         <v>0x68</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>23</v>
@@ -4832,19 +4833,19 @@
         <v>0x69</v>
       </c>
       <c r="B107" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D107" t="s">
+        <v>21</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F107" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E107" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F107" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="G107" s="4" t="s">
         <v>23</v>
@@ -4855,23 +4856,20 @@
         <f t="shared" si="2"/>
         <v>0x6A</v>
       </c>
-      <c r="B108" s="13" t="s">
-        <v>231</v>
+      <c r="B108" s="16" t="s">
+        <v>229</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="D108" t="s">
-        <v>21</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>237</v>
+        <v>228</v>
+      </c>
+      <c r="E108" s="23" t="s">
+        <v>230</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="G108" s="4" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -4879,20 +4877,23 @@
         <f t="shared" si="2"/>
         <v>0x6B</v>
       </c>
-      <c r="B109" s="16" t="s">
-        <v>235</v>
+      <c r="B109" s="13" t="s">
+        <v>224</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D109" t="s">
-        <v>234</v>
-      </c>
-      <c r="E109" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>185</v>
+        <v>226</v>
+      </c>
+      <c r="D109" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G109" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4900,14 +4901,14 @@
         <f t="shared" si="2"/>
         <v>0x6C</v>
       </c>
-      <c r="B110" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D110" s="4" t="s">
-        <v>23</v>
+      <c r="B110" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="C110" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D110" s="24" t="s">
+        <v>228</v>
       </c>
       <c r="E110" s="4" t="s">
         <v>23</v>
@@ -6692,7 +6693,7 @@
       <formula>LEFT(G33,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G110:G257 G2:G41">
+  <conditionalFormatting sqref="G2:G41 G109:G257">
     <cfRule type="containsText" dxfId="134" priority="167" operator="containsText" text="as specified in operand A">
       <formula>NOT(ISERROR(SEARCH("as specified in operand A",G2)))</formula>
     </cfRule>
@@ -7088,76 +7089,76 @@
       <formula>LEFT(D100,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G105:G107 G110:G257 G2:G102">
+  <conditionalFormatting sqref="G104:G106 G2:G101 G109:G257">
     <cfRule type="containsText" dxfId="22" priority="166" operator="containsText" text="bit copy store">
       <formula>NOT(ISERROR(SEARCH("bit copy store",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G103:G104">
+  <conditionalFormatting sqref="G102:G103">
     <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text="bit copy store">
-      <formula>NOT(ISERROR(SEARCH("bit copy store",G103)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bit copy store",G102)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G108">
+  <conditionalFormatting sqref="G107">
     <cfRule type="containsText" dxfId="20" priority="25" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",G108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bit no.",G107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="19" priority="26" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",G108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",G107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="28" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",G108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("byte of constant",G107)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="17" priority="29" operator="beginsWith" text="register">
-      <formula>LEFT(G108,LEN("register"))="register"</formula>
+      <formula>LEFT(G107,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E108:F108 F109">
+  <conditionalFormatting sqref="E107:F107 F108">
     <cfRule type="beginsWith" dxfId="16" priority="6" operator="beginsWith" text="byte ">
-      <formula>LEFT(E108,LEN("byte "))="byte "</formula>
+      <formula>LEFT(E107,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G108">
+  <conditionalFormatting sqref="G107">
     <cfRule type="containsText" dxfId="15" priority="27" operator="containsText" text="bit copy store">
-      <formula>NOT(ISERROR(SEARCH("bit copy store",G108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bit copy store",G107)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E110:G110">
+  <conditionalFormatting sqref="E109:G110">
     <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",E110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bit no.",E109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",E110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",E109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",E110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("byte of constant",E109)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="11" priority="16" operator="beginsWith" text="register">
-      <formula>LEFT(E110,LEN("register"))="register"</formula>
+      <formula>LEFT(E109,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E110:F110">
+  <conditionalFormatting sqref="E109:F110">
     <cfRule type="beginsWith" dxfId="10" priority="11" operator="beginsWith" text="byte ">
-      <formula>LEFT(E110,LEN("byte "))="byte "</formula>
+      <formula>LEFT(E109,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G110">
+  <conditionalFormatting sqref="G109:G110">
     <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="bit copy store">
-      <formula>NOT(ISERROR(SEARCH("bit copy store",G110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bit copy store",G109)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E108:F108 F109">
+  <conditionalFormatting sqref="E107:F107 F108">
     <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",E108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bit no.",E107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",E108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",E107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",E108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("byte of constant",E107)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="5" priority="10" operator="beginsWith" text="register">
-      <formula>LEFT(E108,LEN("register"))="register"</formula>
+      <formula>LEFT(E107,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:F17">

</xml_diff>

<commit_message>
added and implemented a "RUN" command
- also added a sysvarStore in preparation for implementing the get and set instructions
</commit_message>
<xml_diff>
--- a/res/instruction_set.xlsx
+++ b/res/instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukas\git\ArduOS\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4B75AE-D231-499D-99A7-DBAA53AF6375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926EB3C0-6AA5-4211-9F74-72204330EA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B2464EDA-0DBA-4918-93CA-197D58077369}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="252">
   <si>
     <t>Instr. ID</t>
   </si>
@@ -772,6 +772,15 @@
   </si>
   <si>
     <t>opens the next file in the current directory (sets bit copy store to 1 on success, to 0 on failure); will always switch the current file</t>
+  </si>
+  <si>
+    <t>RUN</t>
+  </si>
+  <si>
+    <t>change the currently running program to the one with it's executable path described by the null-terminated string at memory address by reg A &amp; B</t>
+  </si>
+  <si>
+    <t>register B (most significant byte)</t>
   </si>
 </sst>
 </file>
@@ -2270,8 +2279,8 @@
   </sheetPr>
   <dimension ref="A1:H257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4925,10 +4934,18 @@
         <f t="shared" si="2"/>
         <v>0x6D</v>
       </c>
-      <c r="B111" s="13"/>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
-      <c r="E111" s="3"/>
+      <c r="B111" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>251</v>
+      </c>
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
     </row>

</xml_diff>

<commit_message>
finished the implementation of the runtime for the Arduino UNO
</commit_message>
<xml_diff>
--- a/res/instruction_set.xlsx
+++ b/res/instruction_set.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukas\git\ArduOS\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926EB3C0-6AA5-4211-9F74-72204330EA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1E3C21-9590-4715-87B0-11E2167E738D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B2464EDA-0DBA-4918-93CA-197D58077369}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B2464EDA-0DBA-4918-93CA-197D58077369}"/>
   </bookViews>
   <sheets>
     <sheet name="instruction set" sheetId="1" r:id="rId1"/>
+    <sheet name="sysvars" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="265">
   <si>
     <t>Instr. ID</t>
   </si>
@@ -781,13 +785,52 @@
   </si>
   <si>
     <t>register B (most significant byte)</t>
+  </si>
+  <si>
+    <t>Sysvar ID</t>
+  </si>
+  <si>
+    <t>meaning</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>free system memory (physical RAM)</t>
+  </si>
+  <si>
+    <t>screen width</t>
+  </si>
+  <si>
+    <t>screen height</t>
+  </si>
+  <si>
+    <t>x-offset</t>
+  </si>
+  <si>
+    <t>y-offset</t>
+  </si>
+  <si>
+    <t>screen width modifier</t>
+  </si>
+  <si>
+    <t>screen height modifier</t>
+  </si>
+  <si>
+    <t>currently used file (value must either be 1 or 2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -805,6 +848,27 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -960,7 +1024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1000,11 +1064,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="137">
+  <dxfs count="139">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2279,7 +2367,7 @@
   </sheetPr>
   <dimension ref="A1:H257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+    <sheetView topLeftCell="A96" workbookViewId="0">
       <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
@@ -6703,503 +6791,661 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G33">
-    <cfRule type="containsText" dxfId="136" priority="168" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="138" priority="168" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G33)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="135" priority="169" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="137" priority="169" operator="beginsWith" text="register">
       <formula>LEFT(G33,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G41 G109:G257">
-    <cfRule type="containsText" dxfId="134" priority="167" operator="containsText" text="as specified in operand A">
+    <cfRule type="containsText" dxfId="136" priority="167" operator="containsText" text="as specified in operand A">
       <formula>NOT(ISERROR(SEARCH("as specified in operand A",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="170" operator="containsText" text="equality, less/greater than">
+    <cfRule type="containsText" dxfId="135" priority="170" operator="containsText" text="equality, less/greater than">
       <formula>NOT(ISERROR(SEARCH("equality, less/greater than",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="171" operator="containsText" text="carry">
+    <cfRule type="containsText" dxfId="134" priority="171" operator="containsText" text="carry">
       <formula>NOT(ISERROR(SEARCH("carry",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37:G41">
-    <cfRule type="containsText" dxfId="131" priority="162" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="133" priority="162" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G37)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="130" priority="163" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="132" priority="163" operator="beginsWith" text="register">
       <formula>LEFT(G37,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46 G74:G76">
-    <cfRule type="containsText" dxfId="129" priority="158" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="131" priority="158" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="159" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="130" priority="159" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="160" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="129" priority="160" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G46)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="126" priority="161" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="128" priority="161" operator="beginsWith" text="register">
       <formula>LEFT(G46,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47">
-    <cfRule type="containsText" dxfId="125" priority="154" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="127" priority="154" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="155" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="126" priority="155" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="156" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="125" priority="156" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G47)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="122" priority="157" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="124" priority="157" operator="beginsWith" text="register">
       <formula>LEFT(G47,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48:G49">
-    <cfRule type="containsText" dxfId="121" priority="150" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="123" priority="150" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="151" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="122" priority="151" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="152" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="121" priority="152" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G48)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="118" priority="153" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="120" priority="153" operator="beginsWith" text="register">
       <formula>LEFT(G48,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="containsText" dxfId="117" priority="146" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="119" priority="146" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="147" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="118" priority="147" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="148" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="117" priority="148" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G50)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="114" priority="149" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="116" priority="149" operator="beginsWith" text="register">
       <formula>LEFT(G50,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="113" priority="142" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="115" priority="142" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="143" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="114" priority="143" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="144" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="113" priority="144" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G51)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="110" priority="145" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="112" priority="145" operator="beginsWith" text="register">
       <formula>LEFT(G51,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="containsText" dxfId="109" priority="138" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="111" priority="138" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="139" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="110" priority="139" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="140" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="109" priority="140" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G52)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="106" priority="141" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="108" priority="141" operator="beginsWith" text="register">
       <formula>LEFT(G52,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G53">
-    <cfRule type="containsText" dxfId="105" priority="134" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="107" priority="134" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="135" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="106" priority="135" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="136" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="105" priority="136" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G53)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="102" priority="137" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="104" priority="137" operator="beginsWith" text="register">
       <formula>LEFT(G53,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54:G61">
-    <cfRule type="containsText" dxfId="101" priority="130" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="103" priority="130" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="131" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="102" priority="131" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="132" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="101" priority="132" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G54)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="98" priority="133" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="100" priority="133" operator="beginsWith" text="register">
       <formula>LEFT(G54,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62:F62">
-    <cfRule type="containsText" dxfId="97" priority="126" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="99" priority="126" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="127" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="98" priority="127" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="128" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="97" priority="128" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D62)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="94" priority="129" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="96" priority="129" operator="beginsWith" text="register">
       <formula>LEFT(D62,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="containsText" dxfId="93" priority="122" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="95" priority="122" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="123" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="94" priority="123" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="124" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="93" priority="124" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G62)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="90" priority="125" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="92" priority="125" operator="beginsWith" text="register">
       <formula>LEFT(G62,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63:F63">
-    <cfRule type="containsText" dxfId="89" priority="118" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="91" priority="118" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="119" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="90" priority="119" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="120" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="89" priority="120" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D63)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="86" priority="121" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="88" priority="121" operator="beginsWith" text="register">
       <formula>LEFT(D63,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G63">
-    <cfRule type="containsText" dxfId="85" priority="114" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="87" priority="114" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="115" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="86" priority="115" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="116" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="85" priority="116" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G63)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="82" priority="117" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="84" priority="117" operator="beginsWith" text="register">
       <formula>LEFT(G63,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64:F64">
-    <cfRule type="containsText" dxfId="81" priority="110" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="83" priority="110" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="111" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="82" priority="111" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="112" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="81" priority="112" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D64)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="78" priority="113" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="80" priority="113" operator="beginsWith" text="register">
       <formula>LEFT(D64,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G64">
-    <cfRule type="containsText" dxfId="77" priority="106" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="79" priority="106" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="107" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="78" priority="107" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="108" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="77" priority="108" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G64)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="74" priority="109" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="76" priority="109" operator="beginsWith" text="register">
       <formula>LEFT(G64,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:F65">
-    <cfRule type="containsText" dxfId="73" priority="102" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="75" priority="102" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="103" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="74" priority="103" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="104" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="73" priority="104" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D65)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="70" priority="105" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="72" priority="105" operator="beginsWith" text="register">
       <formula>LEFT(D65,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G65">
-    <cfRule type="containsText" dxfId="69" priority="98" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="71" priority="98" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="99" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="70" priority="99" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="100" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="69" priority="100" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G65)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="66" priority="101" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="68" priority="101" operator="beginsWith" text="register">
       <formula>LEFT(G65,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D66:F66">
-    <cfRule type="containsText" dxfId="65" priority="94" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="67" priority="94" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="95" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="66" priority="95" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="96" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="65" priority="96" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D66)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="62" priority="97" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="64" priority="97" operator="beginsWith" text="register">
       <formula>LEFT(D66,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G66:G73">
-    <cfRule type="containsText" dxfId="61" priority="90" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="63" priority="90" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="91" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="62" priority="91" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="92" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="61" priority="92" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G66)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="58" priority="93" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="60" priority="93" operator="beginsWith" text="register">
       <formula>LEFT(G66,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F67:F72">
-    <cfRule type="containsText" dxfId="57" priority="86" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="59" priority="86" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",F67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="87" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="58" priority="87" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",F67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="88" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="57" priority="88" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",F67)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="54" priority="89" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="56" priority="89" operator="beginsWith" text="register">
       <formula>LEFT(F67,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G77:G80">
-    <cfRule type="containsText" dxfId="53" priority="78" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="55" priority="78" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G77)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="79" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="54" priority="79" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G77)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="80" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="53" priority="80" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G77)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="50" priority="81" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="52" priority="81" operator="beginsWith" text="register">
       <formula>LEFT(G77,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G93">
-    <cfRule type="containsText" dxfId="49" priority="58" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="51" priority="58" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="59" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="50" priority="59" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="60" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="49" priority="60" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G93)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="61" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="48" priority="61" operator="beginsWith" text="register">
       <formula>LEFT(G93,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E94:G97">
-    <cfRule type="containsText" dxfId="45" priority="54" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="47" priority="54" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",E94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="55" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="46" priority="55" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",E94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="56" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="45" priority="56" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",E94)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="42" priority="57" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="44" priority="57" operator="beginsWith" text="register">
       <formula>LEFT(E94,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D95:D96">
-    <cfRule type="containsText" dxfId="41" priority="50" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="43" priority="50" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="51" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="42" priority="51" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="52" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="41" priority="52" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D95)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="38" priority="53" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="40" priority="53" operator="beginsWith" text="register">
       <formula>LEFT(D95,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:F257">
-    <cfRule type="beginsWith" dxfId="37" priority="41" operator="beginsWith" text="byte ">
+    <cfRule type="beginsWith" dxfId="39" priority="41" operator="beginsWith" text="byte ">
       <formula>LEFT(D2,LEN("byte "))="byte "</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="164" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="38" priority="164" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="165" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="37" priority="165" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="176" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="36" priority="176" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D2)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="33" priority="179" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="35" priority="179" operator="beginsWith" text="register">
       <formula>LEFT(D2,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E99:F99">
-    <cfRule type="containsText" dxfId="32" priority="37" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="34" priority="37" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",E99)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="38" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="33" priority="38" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",E99)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="39" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="32" priority="39" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",E99)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="29" priority="40" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="31" priority="40" operator="beginsWith" text="register">
       <formula>LEFT(E99,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E99:F99">
-    <cfRule type="beginsWith" dxfId="28" priority="36" operator="beginsWith" text="byte ">
+    <cfRule type="beginsWith" dxfId="30" priority="36" operator="beginsWith" text="byte ">
       <formula>LEFT(E99,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D100:F100">
-    <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="33" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="34" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="27" priority="34" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D100)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="35" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="26" priority="35" operator="beginsWith" text="register">
       <formula>LEFT(D100,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D100:F100">
-    <cfRule type="beginsWith" dxfId="23" priority="31" operator="beginsWith" text="byte ">
+    <cfRule type="beginsWith" dxfId="25" priority="31" operator="beginsWith" text="byte ">
       <formula>LEFT(D100,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G104:G106 G2:G101 G109:G257">
-    <cfRule type="containsText" dxfId="22" priority="166" operator="containsText" text="bit copy store">
+    <cfRule type="containsText" dxfId="24" priority="166" operator="containsText" text="bit copy store">
       <formula>NOT(ISERROR(SEARCH("bit copy store",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G102:G103">
-    <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text="bit copy store">
+    <cfRule type="containsText" dxfId="23" priority="30" operator="containsText" text="bit copy store">
       <formula>NOT(ISERROR(SEARCH("bit copy store",G102)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G107">
-    <cfRule type="containsText" dxfId="20" priority="25" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="26" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="28" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G107)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="17" priority="29" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="19" priority="29" operator="beginsWith" text="register">
       <formula>LEFT(G107,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107:F107 F108">
-    <cfRule type="beginsWith" dxfId="16" priority="6" operator="beginsWith" text="byte ">
+    <cfRule type="beginsWith" dxfId="18" priority="6" operator="beginsWith" text="byte ">
       <formula>LEFT(E107,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G107">
-    <cfRule type="containsText" dxfId="15" priority="27" operator="containsText" text="bit copy store">
+    <cfRule type="containsText" dxfId="17" priority="27" operator="containsText" text="bit copy store">
       <formula>NOT(ISERROR(SEARCH("bit copy store",G107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109:G110">
-    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",E109)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="11" priority="16" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="13" priority="16" operator="beginsWith" text="register">
       <formula>LEFT(E109,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109:F110">
-    <cfRule type="beginsWith" dxfId="10" priority="11" operator="beginsWith" text="byte ">
+    <cfRule type="beginsWith" dxfId="12" priority="11" operator="beginsWith" text="byte ">
       <formula>LEFT(E109,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G109:G110">
-    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="bit copy store">
+    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="bit copy store">
       <formula>NOT(ISERROR(SEARCH("bit copy store",G109)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107:F107 F108">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",E107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",E107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",E107)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="5" priority="10" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="7" priority="10" operator="beginsWith" text="register">
       <formula>LEFT(E107,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:F17">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:F17">
-    <cfRule type="beginsWith" dxfId="3" priority="1" operator="beginsWith" text="byte ">
+    <cfRule type="beginsWith" dxfId="5" priority="1" operator="beginsWith" text="byte ">
       <formula>LEFT(E16,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:F17">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",E16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="5" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="2" priority="5" operator="beginsWith" text="register">
       <formula>LEFT(E16,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="52" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F4047B-451C-46CD-80A9-81E84D54D184}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="3" max="4" width="3.5703125" style="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
+        <v>0</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="26">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
+        <v>3</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="26">
+        <v>4</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
+        <v>5</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
+        <v>6</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="26">
+        <v>7</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:D1048576">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(C1))=0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="x">
+      <formula>NOT(ISERROR(SEARCH("x",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added a screen oriantation sysvar
</commit_message>
<xml_diff>
--- a/res/instruction_set.xlsx
+++ b/res/instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukas\git\ArduOS\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1E3C21-9590-4715-87B0-11E2167E738D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929EB7AD-8D61-4E5E-BEFC-9D95B36744BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B2464EDA-0DBA-4918-93CA-197D58077369}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="266">
   <si>
     <t>Instr. ID</t>
   </si>
@@ -824,6 +824,9 @@
   </si>
   <si>
     <t>currently used file (value must either be 1 or 2)</t>
+  </si>
+  <si>
+    <t>screen orientation (value must be 0, 1, 2 or 3)</t>
   </si>
 </sst>
 </file>
@@ -888,7 +891,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1020,11 +1023,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1071,6 +1087,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -7297,7 +7315,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7387,14 +7405,14 @@
       <c r="D7" s="28"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="26">
+      <c r="A8" s="32">
         <v>6</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
@@ -7407,10 +7425,14 @@
       <c r="D9" s="28"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
+      <c r="A10" s="31">
+        <v>8</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>

</xml_diff>

<commit_message>
added micros() and millis() to the system variables
</commit_message>
<xml_diff>
--- a/res/instruction_set.xlsx
+++ b/res/instruction_set.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukas\git\ArduOS\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929EB7AD-8D61-4E5E-BEFC-9D95B36744BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A12CA0-9F0C-421D-8580-60AA1C56A032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B2464EDA-0DBA-4918-93CA-197D58077369}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="268">
   <si>
     <t>Instr. ID</t>
   </si>
@@ -827,6 +827,12 @@
   </si>
   <si>
     <t>screen orientation (value must be 0, 1, 2 or 3)</t>
+  </si>
+  <si>
+    <t>result of micros()</t>
+  </si>
+  <si>
+    <t>result of millis()</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1099,24 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="139">
+  <dxfs count="141">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -6809,499 +6832,499 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G33">
-    <cfRule type="containsText" dxfId="138" priority="168" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="140" priority="168" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G33)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="137" priority="169" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="139" priority="169" operator="beginsWith" text="register">
       <formula>LEFT(G33,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G41 G109:G257">
-    <cfRule type="containsText" dxfId="136" priority="167" operator="containsText" text="as specified in operand A">
+    <cfRule type="containsText" dxfId="138" priority="167" operator="containsText" text="as specified in operand A">
       <formula>NOT(ISERROR(SEARCH("as specified in operand A",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="170" operator="containsText" text="equality, less/greater than">
+    <cfRule type="containsText" dxfId="137" priority="170" operator="containsText" text="equality, less/greater than">
       <formula>NOT(ISERROR(SEARCH("equality, less/greater than",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="171" operator="containsText" text="carry">
+    <cfRule type="containsText" dxfId="136" priority="171" operator="containsText" text="carry">
       <formula>NOT(ISERROR(SEARCH("carry",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37:G41">
-    <cfRule type="containsText" dxfId="133" priority="162" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="135" priority="162" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G37)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="132" priority="163" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="134" priority="163" operator="beginsWith" text="register">
       <formula>LEFT(G37,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46 G74:G76">
-    <cfRule type="containsText" dxfId="131" priority="158" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="133" priority="158" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="159" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="132" priority="159" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="160" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="131" priority="160" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G46)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="128" priority="161" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="130" priority="161" operator="beginsWith" text="register">
       <formula>LEFT(G46,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47">
-    <cfRule type="containsText" dxfId="127" priority="154" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="129" priority="154" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="155" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="128" priority="155" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="156" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="127" priority="156" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G47)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="124" priority="157" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="126" priority="157" operator="beginsWith" text="register">
       <formula>LEFT(G47,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48:G49">
-    <cfRule type="containsText" dxfId="123" priority="150" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="125" priority="150" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="151" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="124" priority="151" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="152" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="123" priority="152" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G48)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="120" priority="153" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="122" priority="153" operator="beginsWith" text="register">
       <formula>LEFT(G48,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="containsText" dxfId="119" priority="146" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="121" priority="146" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="147" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="120" priority="147" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="148" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="119" priority="148" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G50)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="116" priority="149" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="118" priority="149" operator="beginsWith" text="register">
       <formula>LEFT(G50,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="115" priority="142" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="117" priority="142" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="143" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="116" priority="143" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="144" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="115" priority="144" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G51)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="112" priority="145" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="114" priority="145" operator="beginsWith" text="register">
       <formula>LEFT(G51,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="containsText" dxfId="111" priority="138" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="113" priority="138" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="139" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="112" priority="139" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="140" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="111" priority="140" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G52)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="108" priority="141" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="110" priority="141" operator="beginsWith" text="register">
       <formula>LEFT(G52,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G53">
-    <cfRule type="containsText" dxfId="107" priority="134" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="109" priority="134" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="135" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="108" priority="135" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="136" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="107" priority="136" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G53)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="104" priority="137" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="106" priority="137" operator="beginsWith" text="register">
       <formula>LEFT(G53,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54:G61">
-    <cfRule type="containsText" dxfId="103" priority="130" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="105" priority="130" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="131" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="104" priority="131" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="132" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="103" priority="132" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G54)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="100" priority="133" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="102" priority="133" operator="beginsWith" text="register">
       <formula>LEFT(G54,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62:F62">
-    <cfRule type="containsText" dxfId="99" priority="126" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="101" priority="126" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="127" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="100" priority="127" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="128" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="99" priority="128" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D62)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="96" priority="129" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="98" priority="129" operator="beginsWith" text="register">
       <formula>LEFT(D62,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="containsText" dxfId="95" priority="122" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="97" priority="122" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="123" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="96" priority="123" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="124" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="95" priority="124" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G62)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="92" priority="125" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="94" priority="125" operator="beginsWith" text="register">
       <formula>LEFT(G62,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63:F63">
-    <cfRule type="containsText" dxfId="91" priority="118" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="93" priority="118" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="119" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="92" priority="119" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="120" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="91" priority="120" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D63)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="88" priority="121" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="90" priority="121" operator="beginsWith" text="register">
       <formula>LEFT(D63,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G63">
-    <cfRule type="containsText" dxfId="87" priority="114" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="89" priority="114" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="115" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="88" priority="115" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="116" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="87" priority="116" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G63)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="84" priority="117" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="86" priority="117" operator="beginsWith" text="register">
       <formula>LEFT(G63,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64:F64">
-    <cfRule type="containsText" dxfId="83" priority="110" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="85" priority="110" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="111" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="84" priority="111" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="112" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="83" priority="112" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D64)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="80" priority="113" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="82" priority="113" operator="beginsWith" text="register">
       <formula>LEFT(D64,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G64">
-    <cfRule type="containsText" dxfId="79" priority="106" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="81" priority="106" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="107" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="80" priority="107" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="108" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="79" priority="108" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G64)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="76" priority="109" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="78" priority="109" operator="beginsWith" text="register">
       <formula>LEFT(G64,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:F65">
-    <cfRule type="containsText" dxfId="75" priority="102" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="77" priority="102" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="103" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="76" priority="103" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="104" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="75" priority="104" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D65)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="72" priority="105" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="74" priority="105" operator="beginsWith" text="register">
       <formula>LEFT(D65,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G65">
-    <cfRule type="containsText" dxfId="71" priority="98" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="73" priority="98" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="99" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="72" priority="99" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="100" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="71" priority="100" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G65)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="68" priority="101" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="70" priority="101" operator="beginsWith" text="register">
       <formula>LEFT(G65,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D66:F66">
-    <cfRule type="containsText" dxfId="67" priority="94" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="69" priority="94" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="95" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="68" priority="95" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="96" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="67" priority="96" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D66)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="64" priority="97" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="66" priority="97" operator="beginsWith" text="register">
       <formula>LEFT(D66,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G66:G73">
-    <cfRule type="containsText" dxfId="63" priority="90" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="65" priority="90" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="91" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="64" priority="91" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G66)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="92" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="63" priority="92" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G66)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="60" priority="93" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="62" priority="93" operator="beginsWith" text="register">
       <formula>LEFT(G66,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F67:F72">
-    <cfRule type="containsText" dxfId="59" priority="86" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="61" priority="86" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",F67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="87" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="60" priority="87" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",F67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="88" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="59" priority="88" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",F67)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="56" priority="89" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="58" priority="89" operator="beginsWith" text="register">
       <formula>LEFT(F67,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G77:G80">
-    <cfRule type="containsText" dxfId="55" priority="78" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="57" priority="78" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G77)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="79" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="56" priority="79" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G77)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="80" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="55" priority="80" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G77)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="52" priority="81" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="54" priority="81" operator="beginsWith" text="register">
       <formula>LEFT(G77,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G93">
-    <cfRule type="containsText" dxfId="51" priority="58" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="53" priority="58" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="59" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="52" priority="59" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="60" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="51" priority="60" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G93)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="48" priority="61" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="50" priority="61" operator="beginsWith" text="register">
       <formula>LEFT(G93,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E94:G97">
-    <cfRule type="containsText" dxfId="47" priority="54" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="49" priority="54" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",E94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="55" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="48" priority="55" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",E94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="56" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="47" priority="56" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",E94)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="44" priority="57" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="46" priority="57" operator="beginsWith" text="register">
       <formula>LEFT(E94,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D95:D96">
-    <cfRule type="containsText" dxfId="43" priority="50" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="45" priority="50" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="51" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="44" priority="51" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="52" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="43" priority="52" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D95)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="40" priority="53" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="42" priority="53" operator="beginsWith" text="register">
       <formula>LEFT(D95,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:F257">
-    <cfRule type="beginsWith" dxfId="39" priority="41" operator="beginsWith" text="byte ">
+    <cfRule type="beginsWith" dxfId="41" priority="41" operator="beginsWith" text="byte ">
       <formula>LEFT(D2,LEN("byte "))="byte "</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="164" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="40" priority="164" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="165" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="39" priority="165" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="176" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="38" priority="176" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D2)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="35" priority="179" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="37" priority="179" operator="beginsWith" text="register">
       <formula>LEFT(D2,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E99:F99">
-    <cfRule type="containsText" dxfId="34" priority="37" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",E99)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="38" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="35" priority="38" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",E99)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="39" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="34" priority="39" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",E99)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="31" priority="40" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="33" priority="40" operator="beginsWith" text="register">
       <formula>LEFT(E99,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E99:F99">
-    <cfRule type="beginsWith" dxfId="30" priority="36" operator="beginsWith" text="byte ">
+    <cfRule type="beginsWith" dxfId="32" priority="36" operator="beginsWith" text="byte ">
       <formula>LEFT(E99,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D100:F100">
-    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",D100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",D100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="34" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="29" priority="34" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",D100)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="35" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="28" priority="35" operator="beginsWith" text="register">
       <formula>LEFT(D100,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D100:F100">
-    <cfRule type="beginsWith" dxfId="25" priority="31" operator="beginsWith" text="byte ">
+    <cfRule type="beginsWith" dxfId="27" priority="31" operator="beginsWith" text="byte ">
       <formula>LEFT(D100,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G104:G106 G2:G101 G109:G257">
-    <cfRule type="containsText" dxfId="24" priority="166" operator="containsText" text="bit copy store">
+    <cfRule type="containsText" dxfId="26" priority="166" operator="containsText" text="bit copy store">
       <formula>NOT(ISERROR(SEARCH("bit copy store",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G102:G103">
-    <cfRule type="containsText" dxfId="23" priority="30" operator="containsText" text="bit copy store">
+    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="bit copy store">
       <formula>NOT(ISERROR(SEARCH("bit copy store",G102)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G107">
-    <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",G107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="23" priority="26" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",G107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="22" priority="28" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",G107)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="29" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="21" priority="29" operator="beginsWith" text="register">
       <formula>LEFT(G107,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107:F107 F108">
-    <cfRule type="beginsWith" dxfId="18" priority="6" operator="beginsWith" text="byte ">
+    <cfRule type="beginsWith" dxfId="20" priority="6" operator="beginsWith" text="byte ">
       <formula>LEFT(E107,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G107">
-    <cfRule type="containsText" dxfId="17" priority="27" operator="containsText" text="bit copy store">
+    <cfRule type="containsText" dxfId="19" priority="27" operator="containsText" text="bit copy store">
       <formula>NOT(ISERROR(SEARCH("bit copy store",G107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109:G110">
-    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",E109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="16" priority="15" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",E109)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="16" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="15" priority="16" operator="beginsWith" text="register">
       <formula>LEFT(E109,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109:F110">
-    <cfRule type="beginsWith" dxfId="12" priority="11" operator="beginsWith" text="byte ">
+    <cfRule type="beginsWith" dxfId="14" priority="11" operator="beginsWith" text="byte ">
       <formula>LEFT(E109,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G109:G110">
-    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="bit copy store">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="bit copy store">
       <formula>NOT(ISERROR(SEARCH("bit copy store",G109)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107:F107 F108">
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",E107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",E107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",E107)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="7" priority="10" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="9" priority="10" operator="beginsWith" text="register">
       <formula>LEFT(E107,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:F17">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="byte of constant">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="byte of constant">
       <formula>NOT(ISERROR(SEARCH("byte of constant",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:F17">
-    <cfRule type="beginsWith" dxfId="5" priority="1" operator="beginsWith" text="byte ">
+    <cfRule type="beginsWith" dxfId="7" priority="1" operator="beginsWith" text="byte ">
       <formula>LEFT(E16,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:F17">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="bit no.">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="flag name/no.">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="flag name/no.">
       <formula>NOT(ISERROR(SEARCH("flag name/no.",E16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="5" operator="beginsWith" text="register">
+    <cfRule type="beginsWith" dxfId="4" priority="5" operator="beginsWith" text="register">
       <formula>LEFT(E16,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7315,7 +7338,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7435,16 +7458,28 @@
       <c r="D10" s="28"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
+      <c r="A11" s="26">
+        <v>9</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
+      <c r="A12" s="26">
+        <v>10</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
@@ -7459,12 +7494,20 @@
       <c r="D14" s="30"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:D1048576">
+  <conditionalFormatting sqref="C1:D10 C13:D1048576">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
+      <formula>LEN(TRIM(C1))=0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="x">
+      <formula>NOT(ISERROR(SEARCH("x",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:D12">
     <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(C1))=0</formula>
+      <formula>LEN(TRIM(C11))=0</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="x">
-      <formula>NOT(ISERROR(SEARCH("x",C1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("x",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed some typos in the comments and documentation
</commit_message>
<xml_diff>
--- a/res/instruction_set.xlsx
+++ b/res/instruction_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukas\git\ArduOS\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A12CA0-9F0C-421D-8580-60AA1C56A032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D609FA-D81B-401E-86E5-553DE4AD8034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B2464EDA-0DBA-4918-93CA-197D58077369}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B2464EDA-0DBA-4918-93CA-197D58077369}"/>
   </bookViews>
   <sheets>
     <sheet name="instruction set" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="367">
   <si>
     <t>Instr. ID</t>
   </si>
@@ -833,6 +833,303 @@
   </si>
   <si>
     <t>result of millis()</t>
+  </si>
+  <si>
+    <t>assembly syntax</t>
+  </si>
+  <si>
+    <t>ADD regA, regB</t>
+  </si>
+  <si>
+    <t>ADC regA, regB</t>
+  </si>
+  <si>
+    <t>ADDI regA, byte1~2</t>
+  </si>
+  <si>
+    <t>ADCI regA, byte1~2</t>
+  </si>
+  <si>
+    <t>SUB regA, regB</t>
+  </si>
+  <si>
+    <t>AND regA, regB</t>
+  </si>
+  <si>
+    <t>XOR regA, regB</t>
+  </si>
+  <si>
+    <t>CMP regA, regB</t>
+  </si>
+  <si>
+    <t>MUL regA, regB</t>
+  </si>
+  <si>
+    <t>MULS regA, regB</t>
+  </si>
+  <si>
+    <t>MULSU regA, regB</t>
+  </si>
+  <si>
+    <t>SUC regA, regB</t>
+  </si>
+  <si>
+    <t>SUBI regA, byte1~2</t>
+  </si>
+  <si>
+    <t>SUCI regA, byte1~2</t>
+  </si>
+  <si>
+    <t>ANDI regA, byte1~2</t>
+  </si>
+  <si>
+    <t>ORI regA, byte1~2</t>
+  </si>
+  <si>
+    <t>XORI regA, byte1~2</t>
+  </si>
+  <si>
+    <t>SBR regA, byte1~2</t>
+  </si>
+  <si>
+    <t>CBR regA, byte1~2</t>
+  </si>
+  <si>
+    <t>CMPI regA, byte1~2</t>
+  </si>
+  <si>
+    <t>OR regA, regB</t>
+  </si>
+  <si>
+    <t>MOV regA, regB</t>
+  </si>
+  <si>
+    <t>COM regA</t>
+  </si>
+  <si>
+    <t>CLR regA</t>
+  </si>
+  <si>
+    <t>SER regA</t>
+  </si>
+  <si>
+    <t>LSL regA</t>
+  </si>
+  <si>
+    <t>LSR regA</t>
+  </si>
+  <si>
+    <t>ROL regA</t>
+  </si>
+  <si>
+    <t>ASR regA</t>
+  </si>
+  <si>
+    <t>SWAP regA</t>
+  </si>
+  <si>
+    <t>NEG regA</t>
+  </si>
+  <si>
+    <t>TST regA</t>
+  </si>
+  <si>
+    <t>PUSH regA</t>
+  </si>
+  <si>
+    <t>POP regA</t>
+  </si>
+  <si>
+    <t>SOUT regA</t>
+  </si>
+  <si>
+    <t>SIN regA</t>
+  </si>
+  <si>
+    <t>ROR regA</t>
+  </si>
+  <si>
+    <t>FSET byte1</t>
+  </si>
+  <si>
+    <t>FCLR byte1</t>
+  </si>
+  <si>
+    <t>SOUTI byte1</t>
+  </si>
+  <si>
+    <t>BST regA, byte1</t>
+  </si>
+  <si>
+    <t>BLD regA, byte1</t>
+  </si>
+  <si>
+    <t>LDI regA, byte~2</t>
+  </si>
+  <si>
+    <t>LDR regA, regB~regC</t>
+  </si>
+  <si>
+    <t>STR regA, regB~regC</t>
+  </si>
+  <si>
+    <t>SEB regA~regB</t>
+  </si>
+  <si>
+    <t>SEBI byte1~3</t>
+  </si>
+  <si>
+    <t>RJMP byte1~3</t>
+  </si>
+  <si>
+    <t>JMP regA~regB</t>
+  </si>
+  <si>
+    <t>JMPI byte1~3</t>
+  </si>
+  <si>
+    <t>CALL regA~regB</t>
+  </si>
+  <si>
+    <t>CALLI byte1~3</t>
+  </si>
+  <si>
+    <t>BREQ byte1~3</t>
+  </si>
+  <si>
+    <t>BRNE byte1~3</t>
+  </si>
+  <si>
+    <t>BRGR byte1~3</t>
+  </si>
+  <si>
+    <t>BRLE byte1~3</t>
+  </si>
+  <si>
+    <t>BREQGR byte1~3</t>
+  </si>
+  <si>
+    <t>BREQLE byte1~3</t>
+  </si>
+  <si>
+    <t>RBREQ regA~B</t>
+  </si>
+  <si>
+    <t>RBRNE regA~B</t>
+  </si>
+  <si>
+    <t>RBRGR regA~B</t>
+  </si>
+  <si>
+    <t>RBRLE regA~B</t>
+  </si>
+  <si>
+    <t>RBREQGR regA~B</t>
+  </si>
+  <si>
+    <t>RBREQLE regA~B</t>
+  </si>
+  <si>
+    <t>PXL regA, regB, regC</t>
+  </si>
+  <si>
+    <t>SCLR regA</t>
+  </si>
+  <si>
+    <t>SCLRI byte1~2</t>
+  </si>
+  <si>
+    <t>TSIZ regA</t>
+  </si>
+  <si>
+    <t>TSIZI byte1</t>
+  </si>
+  <si>
+    <t>TWRAPI byte1</t>
+  </si>
+  <si>
+    <t>TOUTI byte1</t>
+  </si>
+  <si>
+    <t>TCOL regA</t>
+  </si>
+  <si>
+    <t>TWRAP regA</t>
+  </si>
+  <si>
+    <t>TOUT regA</t>
+  </si>
+  <si>
+    <t>TCOLI byte1~2</t>
+  </si>
+  <si>
+    <t>TCOLB regA, regB</t>
+  </si>
+  <si>
+    <t>FAV regA</t>
+  </si>
+  <si>
+    <t>FPEK regA</t>
+  </si>
+  <si>
+    <t>FISDIR regA</t>
+  </si>
+  <si>
+    <t>TCPOS regA, regB</t>
+  </si>
+  <si>
+    <t>IMG regA~B</t>
+  </si>
+  <si>
+    <t>IMGI byte1~3</t>
+  </si>
+  <si>
+    <t>RUN regA~B</t>
+  </si>
+  <si>
+    <t>FEXISTS regA, regB~C</t>
+  </si>
+  <si>
+    <t>FOPEN regA, regB~C</t>
+  </si>
+  <si>
+    <t>FREM regA, regB~C</t>
+  </si>
+  <si>
+    <t>FSEKI byte1~3</t>
+  </si>
+  <si>
+    <t>FOUTI byte1</t>
+  </si>
+  <si>
+    <t>FIN regA</t>
+  </si>
+  <si>
+    <t>GET regA</t>
+  </si>
+  <si>
+    <t>FMKDIR   regA, regB~C</t>
+  </si>
+  <si>
+    <t>FRMDIR regA, regB~C</t>
+  </si>
+  <si>
+    <t>FNAME regA, regB</t>
+  </si>
+  <si>
+    <t>FSEK regA, regB~C</t>
+  </si>
+  <si>
+    <t>FOUT regA</t>
+  </si>
+  <si>
+    <t>SET regA, regB~C</t>
+  </si>
+  <si>
+    <t>SETI byte1, regB~C</t>
+  </si>
+  <si>
+    <t>GETI byte1</t>
   </si>
 </sst>
 </file>
@@ -897,7 +1194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1042,11 +1339,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD9D9D9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1095,6 +1401,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2408,17 +2717,19 @@
   </sheetPr>
   <dimension ref="A1:H257"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="129.7109375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="30.28515625" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" customWidth="1"/>
     <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2443,7 +2754,9 @@
       <c r="G1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="15"/>
+      <c r="H1" s="34" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
@@ -2468,6 +2781,9 @@
       <c r="G2" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="H2" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
@@ -2492,6 +2808,9 @@
       <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="H3" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
@@ -2516,6 +2835,9 @@
       <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="H4" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
@@ -2540,6 +2862,9 @@
       <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="H5" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
@@ -2564,6 +2889,9 @@
       <c r="G6" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="H6" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
@@ -2588,6 +2916,9 @@
       <c r="G7" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="H7" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
@@ -2612,6 +2943,9 @@
       <c r="G8" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="H8" s="17" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="str">
@@ -2636,6 +2970,9 @@
       <c r="G9" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="H9" s="21" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="str">
@@ -2660,6 +2997,9 @@
       <c r="G10" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="H10" s="21" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="str">
@@ -2684,6 +3024,9 @@
       <c r="G11" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="H11" s="21" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="str">
@@ -2708,6 +3051,9 @@
       <c r="G12" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="H12" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="str">
@@ -2732,6 +3078,9 @@
       <c r="G13" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="H13" s="21" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="str">
@@ -2756,6 +3105,9 @@
       <c r="G14" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="H14" s="21" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
@@ -2780,6 +3132,9 @@
       <c r="G15" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="H15" s="21" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
@@ -2804,8 +3159,11 @@
       <c r="G16" s="18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="21" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0xF</v>
@@ -2828,8 +3186,11 @@
       <c r="G17" s="18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="21" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x10</v>
@@ -2852,8 +3213,11 @@
       <c r="G18" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="21" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x11</v>
@@ -2876,8 +3240,11 @@
       <c r="G19" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="21" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x12</v>
@@ -2900,8 +3267,11 @@
       <c r="G20" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="21" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x13</v>
@@ -2924,8 +3294,11 @@
       <c r="G21" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="21" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x14</v>
@@ -2948,8 +3321,11 @@
       <c r="G22" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="21" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x15</v>
@@ -2972,8 +3348,11 @@
       <c r="G23" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="21" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x16</v>
@@ -2996,8 +3375,11 @@
       <c r="G24" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="21" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x17</v>
@@ -3020,8 +3402,11 @@
       <c r="G25" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="21" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x18</v>
@@ -3044,8 +3429,11 @@
       <c r="G26" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="21" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x19</v>
@@ -3068,8 +3456,11 @@
       <c r="G27" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="21" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x1A</v>
@@ -3092,8 +3483,11 @@
       <c r="G28" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="35" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x1B</v>
@@ -3116,8 +3510,11 @@
       <c r="G29" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="35" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x1C</v>
@@ -3140,8 +3537,11 @@
       <c r="G30" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="35" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x1D</v>
@@ -3164,8 +3564,11 @@
       <c r="G31" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x1E</v>
@@ -3188,8 +3591,11 @@
       <c r="G32" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="35" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x1F</v>
@@ -3212,8 +3618,11 @@
       <c r="G33" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="35" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x20</v>
@@ -3236,8 +3645,11 @@
       <c r="G34" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x21</v>
@@ -3260,8 +3672,11 @@
       <c r="G35" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="35" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x22</v>
@@ -3284,8 +3699,11 @@
       <c r="G36" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="35" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x23</v>
@@ -3308,8 +3726,11 @@
       <c r="G37" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="17" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x24</v>
@@ -3332,8 +3753,11 @@
       <c r="G38" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="21" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x25</v>
@@ -3356,8 +3780,11 @@
       <c r="G39" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x26</v>
@@ -3380,8 +3807,11 @@
       <c r="G40" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="21" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x27</v>
@@ -3404,8 +3834,11 @@
       <c r="G41" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="21" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x28</v>
@@ -3428,8 +3861,11 @@
       <c r="G42" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="21" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x29</v>
@@ -3452,8 +3888,11 @@
       <c r="G43" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="35" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x2A</v>
@@ -3476,8 +3915,11 @@
       <c r="G44" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="35" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x2B</v>
@@ -3500,8 +3942,11 @@
       <c r="G45" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="21" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x2C</v>
@@ -3524,8 +3969,11 @@
       <c r="G46" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="35" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x2D</v>
@@ -3548,8 +3996,11 @@
       <c r="G47" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="35" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x2E</v>
@@ -3572,8 +4023,11 @@
       <c r="G48" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="35" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x2F</v>
@@ -3596,8 +4050,11 @@
       <c r="G49" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="17" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x30</v>
@@ -3620,8 +4077,11 @@
       <c r="G50" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" s="17" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x31</v>
@@ -3644,8 +4104,11 @@
       <c r="G51" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" s="21" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x32</v>
@@ -3668,8 +4131,11 @@
       <c r="G52" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="21" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x33</v>
@@ -3692,8 +4158,11 @@
       <c r="G53" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="21" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x34</v>
@@ -3716,8 +4185,11 @@
       <c r="G54" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" s="21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x35</v>
@@ -3740,8 +4212,11 @@
       <c r="G55" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" s="21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x36</v>
@@ -3764,8 +4239,11 @@
       <c r="G56" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" s="35" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x37</v>
@@ -3788,8 +4266,11 @@
       <c r="G57" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57" s="35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x38</v>
@@ -3812,8 +4293,11 @@
       <c r="G58" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" s="35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x39</v>
@@ -3836,8 +4320,11 @@
       <c r="G59" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59" s="35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x3A</v>
@@ -3860,8 +4347,11 @@
       <c r="G60" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60" s="35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x3B</v>
@@ -3884,8 +4374,11 @@
       <c r="G61" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" s="21" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x3C</v>
@@ -3908,8 +4401,11 @@
       <c r="G62" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" s="21" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x3D</v>
@@ -3932,8 +4428,11 @@
       <c r="G63" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63" s="21" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x3E</v>
@@ -3956,8 +4455,11 @@
       <c r="G64" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64" s="21" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x3F</v>
@@ -3980,8 +4482,11 @@
       <c r="G65" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65" s="21" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x40</v>
@@ -4004,8 +4509,11 @@
       <c r="G66" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66" s="21" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x41</v>
@@ -4028,8 +4536,11 @@
       <c r="G67" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67" s="21" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="str">
         <f t="shared" si="1"/>
         <v>0x42</v>
@@ -4052,8 +4563,11 @@
       <c r="G68" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68" s="21" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="str">
         <f t="shared" ref="A69:A132" si="2">CONCATENATE("0x", DEC2HEX(ROW()-2))</f>
         <v>0x43</v>
@@ -4076,8 +4590,11 @@
       <c r="G69" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69" s="21" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x44</v>
@@ -4100,8 +4617,11 @@
       <c r="G70" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70" s="21" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x45</v>
@@ -4124,8 +4644,11 @@
       <c r="G71" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71" s="21" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x46</v>
@@ -4148,8 +4671,11 @@
       <c r="G72" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H72" s="21" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x47</v>
@@ -4172,8 +4698,11 @@
       <c r="G73" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73" s="21" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x48</v>
@@ -4196,8 +4725,11 @@
       <c r="G74" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74" s="21" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x49</v>
@@ -4220,8 +4752,11 @@
       <c r="G75" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75" s="21" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x4A</v>
@@ -4244,8 +4779,11 @@
       <c r="G76" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76" s="21" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x4B</v>
@@ -4268,8 +4806,11 @@
       <c r="G77" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77" s="21" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x4C</v>
@@ -4292,8 +4833,11 @@
       <c r="G78" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78" s="21" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x4D</v>
@@ -4316,8 +4860,11 @@
       <c r="G79" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79" s="21" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x4E</v>
@@ -4340,8 +4887,11 @@
       <c r="G80" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80" s="21" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x4F</v>
@@ -4364,8 +4914,11 @@
       <c r="G81" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H81" s="21" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x50</v>
@@ -4388,8 +4941,11 @@
       <c r="G82" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H82" s="21" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x51</v>
@@ -4412,8 +4968,11 @@
       <c r="G83" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83" s="21" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x52</v>
@@ -4436,8 +4995,11 @@
       <c r="G84" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84" s="21" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x53</v>
@@ -4460,8 +5022,11 @@
       <c r="G85" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x54</v>
@@ -4484,8 +5049,11 @@
       <c r="G86" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86" s="21" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x55</v>
@@ -4508,8 +5076,11 @@
       <c r="G87" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H87" s="21" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x56</v>
@@ -4532,8 +5103,11 @@
       <c r="G88" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88" s="21" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x57</v>
@@ -4556,8 +5130,11 @@
       <c r="G89" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89" s="21" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x58</v>
@@ -4580,8 +5157,11 @@
       <c r="G90" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90" s="21" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x59</v>
@@ -4604,8 +5184,11 @@
       <c r="G91" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H91" s="21" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x5A</v>
@@ -4628,8 +5211,11 @@
       <c r="G92" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92" s="21" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x5B</v>
@@ -4652,8 +5238,11 @@
       <c r="G93" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93" s="21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x5C</v>
@@ -4676,8 +5265,11 @@
       <c r="G94" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94" s="21" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x5D</v>
@@ -4700,8 +5292,11 @@
       <c r="G95" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95" s="21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x5E</v>
@@ -4724,8 +5319,11 @@
       <c r="G96" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H96" s="21" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x5F</v>
@@ -4748,8 +5346,11 @@
       <c r="G97" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H97" s="21" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x60</v>
@@ -4772,8 +5373,11 @@
       <c r="G98" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98" s="21" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x61</v>
@@ -4796,8 +5400,11 @@
       <c r="G99" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H99" s="21" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x62</v>
@@ -4820,8 +5427,11 @@
       <c r="G100" s="22" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100" s="21" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x63</v>
@@ -4844,8 +5454,11 @@
       <c r="G101" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H101" s="21" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x64</v>
@@ -4868,8 +5481,11 @@
       <c r="G102" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H102" s="36" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x65</v>
@@ -4892,8 +5508,11 @@
       <c r="G103" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H103" s="36" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x66</v>
@@ -4916,8 +5535,11 @@
       <c r="G104" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H104" s="35" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x67</v>
@@ -4940,8 +5562,11 @@
       <c r="G105" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H105" s="35" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x68</v>
@@ -4964,8 +5589,11 @@
       <c r="G106" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H106" s="21" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x69</v>
@@ -4988,8 +5616,11 @@
       <c r="G107" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H107" s="17" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x6A</v>
@@ -5009,8 +5640,11 @@
       <c r="F108" s="3" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H108" s="35" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x6B</v>
@@ -5033,8 +5667,11 @@
       <c r="G109" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H109" s="35" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x6C</v>
@@ -5057,8 +5694,11 @@
       <c r="G110" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H110" s="35" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x6D</v>
@@ -5075,10 +5715,15 @@
       <c r="E111" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="F111" s="3"/>
+      <c r="F111" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="G111" s="3"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H111" s="35" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="str">
         <f t="shared" si="2"/>
         <v>0x6E</v>
@@ -7180,7 +7825,7 @@
       <formula>LEFT(D95,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:F257">
+  <conditionalFormatting sqref="H8:H11 H13:H30 H32:H33 H35:H38 H40:H55 D2:F257 H61:H103 H106:H110">
     <cfRule type="beginsWith" dxfId="41" priority="41" operator="beginsWith" text="byte ">
       <formula>LEFT(D2,LEN("byte "))="byte "</formula>
     </cfRule>
@@ -7269,7 +7914,7 @@
       <formula>NOT(ISERROR(SEARCH("bit copy store",G107)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E109:G110">
+  <conditionalFormatting sqref="E109:G110 F111">
     <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="bit no.">
       <formula>NOT(ISERROR(SEARCH("bit no.",E109)))</formula>
     </cfRule>
@@ -7283,7 +7928,7 @@
       <formula>LEFT(E109,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E109:F110">
+  <conditionalFormatting sqref="E109:F110 F111">
     <cfRule type="beginsWith" dxfId="14" priority="11" operator="beginsWith" text="byte ">
       <formula>LEFT(E109,LEN("byte "))="byte "</formula>
     </cfRule>
@@ -7337,7 +7982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F4047B-451C-46CD-80A9-81E84D54D184}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed multiple bugs - fixed a bug where data would always be appended to the RAM file, so that it could not be read anymore - fixed a bug that prevented the text color from being set correctly when using TCOL - added a TFT instruction, but that doesnt work correctly, yet
</commit_message>
<xml_diff>
--- a/res/instruction_set.xlsx
+++ b/res/instruction_set.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukas\git\ArduOS\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D609FA-D81B-401E-86E5-553DE4AD8034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A419B6F8-9ED7-47A6-97E7-CEC74BF00BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B2464EDA-0DBA-4918-93CA-197D58077369}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="369">
   <si>
     <t>Instr. ID</t>
   </si>
@@ -1130,6 +1130,12 @@
   </si>
   <si>
     <t>GETI byte1</t>
+  </si>
+  <si>
+    <t>TFT</t>
+  </si>
+  <si>
+    <t>save the current touch position to registers 0 and 1, the x position to r0 and the y position to r1</t>
   </si>
 </sst>
 </file>
@@ -1352,7 +1358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1404,6 +1410,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2717,8 +2724,8 @@
   </sheetPr>
   <dimension ref="A1:H257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="I112" sqref="I112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5718,7 +5725,9 @@
       <c r="F111" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G111" s="3"/>
+      <c r="G111" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="H111" s="35" t="s">
         <v>351</v>
       </c>
@@ -5728,12 +5737,24 @@
         <f t="shared" si="2"/>
         <v>0x6E</v>
       </c>
-      <c r="B112" s="13"/>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
-      <c r="E112" s="3"/>
-      <c r="F112" s="3"/>
-      <c r="G112" s="3"/>
+      <c r="B112" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G112" s="37" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="str">
@@ -7825,7 +7846,7 @@
       <formula>LEFT(D95,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H11 H13:H30 H32:H33 H35:H38 H40:H55 D2:F257 H61:H103 H106:H110">
+  <conditionalFormatting sqref="H8:H11 H13:H30 H32:H33 H35:H38 H40:H55 H61:H103 H106:H110 D2:F257">
     <cfRule type="beginsWith" dxfId="41" priority="41" operator="beginsWith" text="byte ">
       <formula>LEFT(D2,LEN("byte "))="byte "</formula>
     </cfRule>
@@ -7914,26 +7935,26 @@
       <formula>NOT(ISERROR(SEARCH("bit copy store",G107)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E109:G110 F111">
+  <conditionalFormatting sqref="E109:G110 F111:G111 D112:F112">
     <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="bit no.">
-      <formula>NOT(ISERROR(SEARCH("bit no.",E109)))</formula>
+      <formula>NOT(ISERROR(SEARCH("bit no.",D109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="flag name/no.">
-      <formula>NOT(ISERROR(SEARCH("flag name/no.",E109)))</formula>
+      <formula>NOT(ISERROR(SEARCH("flag name/no.",D109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="15" operator="containsText" text="byte of constant">
-      <formula>NOT(ISERROR(SEARCH("byte of constant",E109)))</formula>
+      <formula>NOT(ISERROR(SEARCH("byte of constant",D109)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="15" priority="16" operator="beginsWith" text="register">
-      <formula>LEFT(E109,LEN("register"))="register"</formula>
+      <formula>LEFT(D109,LEN("register"))="register"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E109:F110 F111">
+  <conditionalFormatting sqref="E109:F110 F111:F112 D112:E112">
     <cfRule type="beginsWith" dxfId="14" priority="11" operator="beginsWith" text="byte ">
-      <formula>LEFT(E109,LEN("byte "))="byte "</formula>
+      <formula>LEFT(D109,LEN("byte "))="byte "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G109:G110">
+  <conditionalFormatting sqref="G109:G111">
     <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="bit copy store">
       <formula>NOT(ISERROR(SEARCH("bit copy store",G109)))</formula>
     </cfRule>

</xml_diff>